<commit_message>
Update lut excel files
</commit_message>
<xml_diff>
--- a/lut_generator_E12_10R10M.xlsx
+++ b/lut_generator_E12_10R10M.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20369"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\shared\Dokumente\codebase\avr-quantizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E09F9E44-528B-4383-B42F-05EB8E5F0121}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6476FE-1160-465C-8094-978B2BC42CAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5860" yWindow="0" windowWidth="36500" windowHeight="18320" xr2:uid="{F31E432E-1247-4F18-8B99-AC2EE1672703}"/>
+    <workbookView xWindow="6830" yWindow="0" windowWidth="36500" windowHeight="18320" xr2:uid="{F31E432E-1247-4F18-8B99-AC2EE1672703}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -452,6 +452,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -464,21 +471,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="5" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52672B51-097A-4F0D-94C8-36FB4DE8AA5D}">
   <dimension ref="A1:R83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -829,29 +829,29 @@
     <row r="2" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="10"/>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="19" t="s">
+      <c r="F3" s="23"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="19" t="s">
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
     </row>
     <row r="4" spans="1:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10"/>
@@ -904,7 +904,7 @@
     <row r="5" spans="1:16" s="10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="14"/>
       <c r="C5" s="15"/>
-      <c r="E5" s="24">
+      <c r="E5" s="20">
         <v>8.1999999999999993</v>
       </c>
       <c r="F5" s="8">
@@ -939,14 +939,14 @@
         <f>IF(L5&lt;&gt;"",L5+COUNT(L:L)&amp;", ","")</f>
         <v xml:space="preserve">18, </v>
       </c>
-      <c r="N5" s="23" t="str">
+      <c r="N5" s="19" t="str">
         <f>IF(J5&lt;&gt;"",J5&amp;", "&amp;IF($H5&lt;&gt;$H6,CHAR(10),""),"")</f>
         <v xml:space="preserve">9, </v>
       </c>
-      <c r="O5" s="23"/>
+      <c r="O5" s="19"/>
       <c r="P5" s="26" t="str">
-        <f>"const uint"&amp;$C$8*8&amp;"_t "&amp;"lut_"&amp;$C$6&amp;"["&amp;COUNT($J:$J)+COUNT($L:$L)&amp;"] PROGMEM ="&amp;CHAR(10)&amp;"{"&amp;CHAR(10)&amp;_xlfn.CONCAT($M:$M)&amp;CHAR(10)&amp;CHAR(10)&amp;_xlfn.CONCAT($N:$N)&amp;"};"</f>
-        <v>const uint8_t lut_E12_10R10M[92] PROGMEM =
+        <f>"const __flash uint"&amp;$C$8*8&amp;"_t "&amp;"lut"&amp;$C$8&amp;"d"&amp;$C$7&amp;"_"&amp;$C$6&amp;"["&amp;COUNT($J:$J)+COUNT($L:$L)&amp;"] ="&amp;CHAR(10)&amp;"{"&amp;CHAR(10)&amp;_xlfn.CONCAT($M:$M)&amp;CHAR(10)&amp;CHAR(10)&amp;_xlfn.CONCAT($N:$N)&amp;"};"</f>
+        <v>const __flash uint8_t lut1d4_E12_10R10M[92] =
 {
 // header
 18, 36, 39, 43, 47, 50, 54, 57, 61, 65, 68, 72, 76, 79, 83, 86, 90, 92, 
@@ -980,7 +980,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="24">
+      <c r="E6" s="20">
         <v>10</v>
       </c>
       <c r="F6" s="8">
@@ -1015,12 +1015,12 @@
         <f>IF(L6&lt;&gt;"",L6+COUNT(L:L)&amp;", ","")</f>
         <v/>
       </c>
-      <c r="N6" s="23" t="str">
+      <c r="N6" s="19" t="str">
         <f>IF(J6&lt;&gt;"",J6&amp;", "&amp;IF($H6&lt;&gt;$H7,CHAR(10),""),"")</f>
         <v xml:space="preserve">11, </v>
       </c>
-      <c r="O6" s="23"/>
-      <c r="P6" s="28"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="27"/>
     </row>
     <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
@@ -1031,7 +1031,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="24">
+      <c r="E7" s="20">
         <v>12</v>
       </c>
       <c r="F7" s="8">
@@ -1066,12 +1066,12 @@
         <f t="shared" ref="M7:M30" si="7">IF(L7&lt;&gt;"",L7+COUNT(L:L)&amp;", ","")</f>
         <v/>
       </c>
-      <c r="N7" s="23" t="str">
+      <c r="N7" s="19" t="str">
         <f t="shared" ref="N7:N69" si="8">IF(J7&lt;&gt;"",J7&amp;", "&amp;IF($H7&lt;&gt;$H8,CHAR(10),""),"")</f>
         <v xml:space="preserve">14, </v>
       </c>
-      <c r="O7" s="23"/>
-      <c r="P7" s="28"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="27"/>
     </row>
     <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
@@ -1082,7 +1082,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="24">
+      <c r="E8" s="20">
         <v>15</v>
       </c>
       <c r="F8" s="8">
@@ -1117,12 +1117,12 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N8" s="23" t="str">
+      <c r="N8" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">17, </v>
       </c>
-      <c r="O8" s="23"/>
-      <c r="P8" s="28"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="27"/>
     </row>
     <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
@@ -1133,7 +1133,7 @@
         <v>16</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="24">
+      <c r="E9" s="20">
         <v>18</v>
       </c>
       <c r="F9" s="8">
@@ -1168,19 +1168,19 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N9" s="23" t="str">
+      <c r="N9" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">20, </v>
       </c>
-      <c r="O9" s="23"/>
-      <c r="P9" s="28"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="27"/>
     </row>
     <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="3"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="24">
+      <c r="E10" s="20">
         <v>22</v>
       </c>
       <c r="F10" s="8">
@@ -1215,19 +1215,19 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N10" s="23" t="str">
+      <c r="N10" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">25, </v>
       </c>
-      <c r="O10" s="23"/>
-      <c r="P10" s="28"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="27"/>
     </row>
     <row r="11" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="3"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="24">
+      <c r="E11" s="20">
         <v>27</v>
       </c>
       <c r="F11" s="8">
@@ -1262,21 +1262,21 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N11" s="23" t="str">
+      <c r="N11" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">30, </v>
       </c>
-      <c r="O11" s="23"/>
-      <c r="P11" s="28"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="27"/>
     </row>
     <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="24">
+      <c r="E12" s="20">
         <v>33</v>
       </c>
       <c r="F12" s="8">
@@ -1311,12 +1311,12 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N12" s="23" t="str">
+      <c r="N12" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">36, </v>
       </c>
-      <c r="O12" s="23"/>
-      <c r="P12" s="28"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="27"/>
     </row>
     <row r="13" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
@@ -1328,7 +1328,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="7"/>
-      <c r="E13" s="24">
+      <c r="E13" s="20">
         <v>39</v>
       </c>
       <c r="F13" s="8">
@@ -1363,19 +1363,19 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N13" s="23" t="str">
+      <c r="N13" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">43, </v>
       </c>
-      <c r="O13" s="23"/>
-      <c r="P13" s="28"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="27"/>
     </row>
     <row r="14" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7"/>
       <c r="B14" s="3"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="24">
+      <c r="E14" s="20">
         <v>47</v>
       </c>
       <c r="F14" s="8">
@@ -1410,21 +1410,21 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N14" s="23" t="str">
+      <c r="N14" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">52, </v>
       </c>
-      <c r="O14" s="23"/>
-      <c r="P14" s="28"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="27"/>
     </row>
     <row r="15" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="24">
+      <c r="E15" s="20">
         <v>56</v>
       </c>
       <c r="F15" s="8">
@@ -1459,18 +1459,18 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N15" s="23" t="str">
+      <c r="N15" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">62, </v>
       </c>
-      <c r="O15" s="23"/>
-      <c r="P15" s="28"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="27"/>
     </row>
     <row r="16" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
-      <c r="B16" s="27" t="str">
+      <c r="B16" s="28" t="str">
         <f>$P$5</f>
-        <v>const uint8_t lut_E12_10R10M[92] PROGMEM =
+        <v>const __flash uint8_t lut1d4_E12_10R10M[92] =
 {
 // header
 18, 36, 39, 43, 47, 50, 54, 57, 61, 65, 68, 72, 76, 79, 83, 86, 90, 92, 
@@ -1494,9 +1494,9 @@
 139, 168, 
 };</v>
       </c>
-      <c r="C16" s="27"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="24">
+      <c r="E16" s="20">
         <v>68</v>
       </c>
       <c r="F16" s="8">
@@ -1531,19 +1531,19 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N16" s="23" t="str">
+      <c r="N16" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">75, </v>
       </c>
-      <c r="O16" s="23"/>
-      <c r="P16" s="28"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="27"/>
     </row>
     <row r="17" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
       <c r="B17" s="3"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="24">
+      <c r="E17" s="20">
         <v>82</v>
       </c>
       <c r="F17" s="8">
@@ -1578,19 +1578,19 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N17" s="23" t="str">
+      <c r="N17" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">91, </v>
       </c>
-      <c r="O17" s="23"/>
-      <c r="P17" s="28"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="27"/>
     </row>
     <row r="18" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7"/>
       <c r="B18" s="3"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="24">
+      <c r="E18" s="20">
         <v>100</v>
       </c>
       <c r="F18" s="8">
@@ -1625,19 +1625,19 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N18" s="23" t="str">
+      <c r="N18" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">110, </v>
       </c>
-      <c r="O18" s="23"/>
-      <c r="P18" s="28"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="27"/>
     </row>
     <row r="19" spans="1:16" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7"/>
       <c r="B19" s="3"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="24">
+      <c r="E19" s="20">
         <v>120</v>
       </c>
       <c r="F19" s="8">
@@ -1672,19 +1672,19 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N19" s="23" t="str">
+      <c r="N19" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">135, </v>
       </c>
-      <c r="O19" s="23"/>
-      <c r="P19" s="28"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="27"/>
     </row>
     <row r="20" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
       <c r="B20" s="3"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="24">
+      <c r="E20" s="20">
         <v>150</v>
       </c>
       <c r="F20" s="8">
@@ -1719,19 +1719,19 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N20" s="23" t="str">
+      <c r="N20" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">165, </v>
       </c>
-      <c r="O20" s="23"/>
-      <c r="P20" s="28"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="27"/>
     </row>
     <row r="21" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7"/>
       <c r="B21" s="3"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="24">
+      <c r="E21" s="20">
         <v>180</v>
       </c>
       <c r="F21" s="8">
@@ -1766,19 +1766,19 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N21" s="23" t="str">
+      <c r="N21" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">200, </v>
       </c>
-      <c r="O21" s="23"/>
-      <c r="P21" s="28"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="27"/>
     </row>
     <row r="22" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7"/>
       <c r="B22" s="3"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="24">
+      <c r="E22" s="20">
         <v>220</v>
       </c>
       <c r="F22" s="8">
@@ -1813,20 +1813,20 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N22" s="23" t="str">
+      <c r="N22" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">245, 
 </v>
       </c>
-      <c r="O22" s="23"/>
-      <c r="P22" s="28"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="27"/>
     </row>
     <row r="23" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7"/>
       <c r="B23" s="3"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
-      <c r="E23" s="24">
+      <c r="E23" s="20">
         <v>270</v>
       </c>
       <c r="F23" s="8">
@@ -1861,19 +1861,19 @@
         <f t="shared" si="7"/>
         <v xml:space="preserve">36, </v>
       </c>
-      <c r="N23" s="23" t="str">
+      <c r="N23" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">150, </v>
       </c>
-      <c r="O23" s="23"/>
-      <c r="P23" s="28"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="27"/>
     </row>
     <row r="24" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7"/>
       <c r="B24" s="3"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
-      <c r="E24" s="24">
+      <c r="E24" s="20">
         <v>330</v>
       </c>
       <c r="F24" s="8">
@@ -1908,19 +1908,19 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N24" s="23" t="str">
+      <c r="N24" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">180, </v>
       </c>
-      <c r="O24" s="23"/>
-      <c r="P24" s="28"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="27"/>
     </row>
     <row r="25" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7"/>
       <c r="B25" s="3"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="24">
+      <c r="E25" s="20">
         <v>390</v>
       </c>
       <c r="F25" s="8">
@@ -1955,20 +1955,20 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N25" s="23" t="str">
+      <c r="N25" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">215, 
 </v>
       </c>
-      <c r="O25" s="23"/>
-      <c r="P25" s="28"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="27"/>
     </row>
     <row r="26" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7"/>
       <c r="B26" s="3"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
-      <c r="E26" s="24">
+      <c r="E26" s="20">
         <v>470</v>
       </c>
       <c r="F26" s="8">
@@ -2003,19 +2003,19 @@
         <f t="shared" si="7"/>
         <v xml:space="preserve">39, </v>
       </c>
-      <c r="N26" s="23" t="str">
+      <c r="N26" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">129, </v>
       </c>
-      <c r="O26" s="23"/>
-      <c r="P26" s="28"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="27"/>
     </row>
     <row r="27" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7"/>
       <c r="B27" s="3"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="24">
+      <c r="E27" s="20">
         <v>560</v>
       </c>
       <c r="F27" s="8">
@@ -2050,19 +2050,19 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N27" s="23" t="str">
+      <c r="N27" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">155, </v>
       </c>
-      <c r="O27" s="23"/>
-      <c r="P27" s="28"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="27"/>
     </row>
     <row r="28" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7"/>
       <c r="B28" s="3"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
-      <c r="E28" s="24">
+      <c r="E28" s="20">
         <v>680</v>
       </c>
       <c r="F28" s="8">
@@ -2097,19 +2097,19 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N28" s="23" t="str">
+      <c r="N28" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">188, </v>
       </c>
-      <c r="O28" s="23"/>
-      <c r="P28" s="28"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="27"/>
     </row>
     <row r="29" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="7"/>
       <c r="B29" s="3"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
-      <c r="E29" s="24">
+      <c r="E29" s="20">
         <v>820</v>
       </c>
       <c r="F29" s="8">
@@ -2144,20 +2144,20 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="N29" s="23" t="str">
+      <c r="N29" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">228, 
 </v>
       </c>
-      <c r="O29" s="23"/>
-      <c r="P29" s="28"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="27"/>
     </row>
     <row r="30" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7"/>
       <c r="B30" s="3"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
-      <c r="E30" s="24">
+      <c r="E30" s="20">
         <v>1000</v>
       </c>
       <c r="F30" s="8">
@@ -2192,19 +2192,19 @@
         <f t="shared" si="7"/>
         <v xml:space="preserve">43, </v>
       </c>
-      <c r="N30" s="23" t="str">
+      <c r="N30" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">138, </v>
       </c>
-      <c r="O30" s="23"/>
-      <c r="P30" s="28"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="27"/>
     </row>
     <row r="31" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="7"/>
       <c r="B31" s="3"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
-      <c r="E31" s="24">
+      <c r="E31" s="20">
         <v>1200</v>
       </c>
       <c r="F31" s="8">
@@ -2236,22 +2236,22 @@
         <v/>
       </c>
       <c r="M31" s="7" t="str">
-        <f>IF(L31&lt;&gt;"",L31+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N31" s="23" t="str">
+        <f t="shared" ref="M31:M62" si="9">IF(L31&lt;&gt;"",L31+COUNT(L:L)&amp;", ","")</f>
+        <v/>
+      </c>
+      <c r="N31" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">169, </v>
       </c>
-      <c r="O31" s="23"/>
-      <c r="P31" s="28"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="27"/>
     </row>
     <row r="32" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7"/>
       <c r="B32" s="3"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
-      <c r="E32" s="24">
+      <c r="E32" s="20">
         <v>1500</v>
       </c>
       <c r="F32" s="8">
@@ -2283,22 +2283,22 @@
         <v/>
       </c>
       <c r="M32" s="7" t="str">
-        <f>IF(L32&lt;&gt;"",L32+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N32" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N32" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">206, </v>
       </c>
-      <c r="O32" s="23"/>
-      <c r="P32" s="28"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="27"/>
     </row>
     <row r="33" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7"/>
       <c r="B33" s="3"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
-      <c r="E33" s="24">
+      <c r="E33" s="20">
         <v>1800</v>
       </c>
       <c r="F33" s="8">
@@ -2330,24 +2330,24 @@
         <v/>
       </c>
       <c r="M33" s="7" t="str">
-        <f>IF(L33&lt;&gt;"",L33+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N33" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N33" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">250, 
 </v>
       </c>
-      <c r="O33" s="23"/>
-      <c r="P33" s="28"/>
-      <c r="R33" s="25"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="27"/>
+      <c r="R33" s="21"/>
     </row>
     <row r="34" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="6"/>
       <c r="B34" s="3"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
-      <c r="E34" s="24">
+      <c r="E34" s="20">
         <v>2200</v>
       </c>
       <c r="F34" s="8">
@@ -2379,22 +2379,22 @@
         <v>29</v>
       </c>
       <c r="M34" s="7" t="str">
-        <f>IF(L34&lt;&gt;"",L34+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">47, </v>
       </c>
-      <c r="N34" s="23" t="str">
+      <c r="N34" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">153, </v>
       </c>
-      <c r="O34" s="23"/>
-      <c r="P34" s="28"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="27"/>
     </row>
     <row r="35" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6"/>
       <c r="B35" s="3"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="24">
+      <c r="E35" s="20">
         <v>2700</v>
       </c>
       <c r="F35" s="8">
@@ -2426,22 +2426,22 @@
         <v/>
       </c>
       <c r="M35" s="7" t="str">
-        <f>IF(L35&lt;&gt;"",L35+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N35" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N35" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">188, </v>
       </c>
-      <c r="O35" s="23"/>
-      <c r="P35" s="28"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="27"/>
     </row>
     <row r="36" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" s="3"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="24">
+      <c r="E36" s="20">
         <v>3300</v>
       </c>
       <c r="F36" s="8">
@@ -2473,21 +2473,21 @@
         <v/>
       </c>
       <c r="M36" s="7" t="str">
-        <f>IF(L36&lt;&gt;"",L36+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N36" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N36" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">225, 
 </v>
       </c>
-      <c r="O36" s="23"/>
-      <c r="P36" s="28"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="27"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B37" s="3"/>
       <c r="C37" s="7"/>
-      <c r="E37" s="24">
+      <c r="E37" s="20">
         <v>3900</v>
       </c>
       <c r="F37" s="8">
@@ -2519,20 +2519,20 @@
         <v>32</v>
       </c>
       <c r="M37" s="7" t="str">
-        <f>IF(L37&lt;&gt;"",L37+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">50, </v>
       </c>
-      <c r="N37" s="23" t="str">
+      <c r="N37" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">134, </v>
       </c>
-      <c r="O37" s="23"/>
-      <c r="P37" s="28"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="27"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B38" s="3"/>
       <c r="C38" s="7"/>
-      <c r="E38" s="24">
+      <c r="E38" s="20">
         <v>4700</v>
       </c>
       <c r="F38" s="8">
@@ -2564,20 +2564,20 @@
         <v/>
       </c>
       <c r="M38" s="7" t="str">
-        <f>IF(L38&lt;&gt;"",L38+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N38" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N38" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">161, </v>
       </c>
-      <c r="O38" s="23"/>
-      <c r="P38" s="28"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="27"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B39" s="3"/>
       <c r="C39" s="7"/>
-      <c r="E39" s="24">
+      <c r="E39" s="20">
         <v>5600</v>
       </c>
       <c r="F39" s="8">
@@ -2609,19 +2609,19 @@
         <v/>
       </c>
       <c r="M39" s="7" t="str">
-        <f>IF(L39&lt;&gt;"",L39+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N39" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N39" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">194, </v>
       </c>
-      <c r="O39" s="23"/>
-      <c r="P39" s="28"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="27"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C40" s="7"/>
-      <c r="E40" s="24">
+      <c r="E40" s="20">
         <v>6800</v>
       </c>
       <c r="F40" s="8">
@@ -2653,19 +2653,19 @@
         <v/>
       </c>
       <c r="M40" s="7" t="str">
-        <f>IF(L40&lt;&gt;"",L40+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N40" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N40" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">234, 
 </v>
       </c>
-      <c r="O40" s="23"/>
-      <c r="P40" s="28"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="27"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E41" s="24">
+      <c r="E41" s="20">
         <v>8200</v>
       </c>
       <c r="F41" s="8">
@@ -2697,18 +2697,18 @@
         <v>36</v>
       </c>
       <c r="M41" s="7" t="str">
-        <f>IF(L41&lt;&gt;"",L41+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">54, </v>
       </c>
-      <c r="N41" s="23" t="str">
+      <c r="N41" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">142, </v>
       </c>
-      <c r="O41" s="23"/>
-      <c r="P41" s="28"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="27"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E42" s="24">
+      <c r="E42" s="20">
         <v>10000</v>
       </c>
       <c r="F42" s="8">
@@ -2740,18 +2740,18 @@
         <v/>
       </c>
       <c r="M42" s="7" t="str">
-        <f>IF(L42&lt;&gt;"",L42+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N42" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N42" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">172, </v>
       </c>
-      <c r="O42" s="23"/>
-      <c r="P42" s="28"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="27"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E43" s="24">
+      <c r="E43" s="20">
         <v>12000</v>
       </c>
       <c r="F43" s="8">
@@ -2783,19 +2783,19 @@
         <v/>
       </c>
       <c r="M43" s="7" t="str">
-        <f>IF(L43&lt;&gt;"",L43+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N43" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N43" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">211, 
 </v>
       </c>
-      <c r="O43" s="23"/>
-      <c r="P43" s="28"/>
+      <c r="O43" s="19"/>
+      <c r="P43" s="27"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E44" s="24">
+      <c r="E44" s="20">
         <v>15000</v>
       </c>
       <c r="F44" s="8">
@@ -2827,17 +2827,17 @@
         <v>39</v>
       </c>
       <c r="M44" s="7" t="str">
-        <f>IF(L44&lt;&gt;"",L44+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">57, </v>
       </c>
-      <c r="N44" s="23" t="str">
+      <c r="N44" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">129, </v>
       </c>
       <c r="O44" s="6"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E45" s="24">
+      <c r="E45" s="20">
         <v>18000</v>
       </c>
       <c r="F45" s="8">
@@ -2869,17 +2869,17 @@
         <v/>
       </c>
       <c r="M45" s="7" t="str">
-        <f>IF(L45&lt;&gt;"",L45+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N45" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N45" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">156, </v>
       </c>
       <c r="O45" s="6"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E46" s="24">
+      <c r="E46" s="20">
         <v>22000</v>
       </c>
       <c r="F46" s="8">
@@ -2911,16 +2911,16 @@
         <v/>
       </c>
       <c r="M46" s="7" t="str">
-        <f>IF(L46&lt;&gt;"",L46+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N46" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N46" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">191, </v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E47" s="24">
+      <c r="E47" s="20">
         <v>27000</v>
       </c>
       <c r="F47" s="8">
@@ -2952,17 +2952,17 @@
         <v/>
       </c>
       <c r="M47" s="7" t="str">
-        <f>IF(L47&lt;&gt;"",L47+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N47" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N47" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">234, 
 </v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="E48" s="24">
+      <c r="E48" s="20">
         <v>33000</v>
       </c>
       <c r="F48" s="8">
@@ -2994,17 +2994,17 @@
         <v>43</v>
       </c>
       <c r="M48" s="7" t="str">
-        <f>IF(L48&lt;&gt;"",L48+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">61, </v>
       </c>
-      <c r="N48" s="23" t="str">
+      <c r="N48" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">141, </v>
       </c>
       <c r="O48" s="6"/>
     </row>
     <row r="49" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E49" s="24">
+      <c r="E49" s="20">
         <v>39000</v>
       </c>
       <c r="F49" s="8">
@@ -3036,16 +3036,16 @@
         <v/>
       </c>
       <c r="M49" s="7" t="str">
-        <f>IF(L49&lt;&gt;"",L49+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N49" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N49" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">168, </v>
       </c>
     </row>
     <row r="50" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E50" s="24">
+      <c r="E50" s="20">
         <v>47000</v>
       </c>
       <c r="F50" s="8">
@@ -3077,16 +3077,16 @@
         <v/>
       </c>
       <c r="M50" s="7" t="str">
-        <f>IF(L50&lt;&gt;"",L50+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N50" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N50" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">201, </v>
       </c>
     </row>
     <row r="51" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E51" s="24">
+      <c r="E51" s="20">
         <v>56000</v>
       </c>
       <c r="F51" s="8">
@@ -3118,17 +3118,17 @@
         <v/>
       </c>
       <c r="M51" s="7" t="str">
-        <f>IF(L51&lt;&gt;"",L51+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N51" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N51" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">242, 
 </v>
       </c>
     </row>
     <row r="52" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E52" s="24">
+      <c r="E52" s="20">
         <v>68000</v>
       </c>
       <c r="F52" s="8">
@@ -3160,16 +3160,16 @@
         <v>47</v>
       </c>
       <c r="M52" s="7" t="str">
-        <f>IF(L52&lt;&gt;"",L52+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">65, </v>
       </c>
-      <c r="N52" s="23" t="str">
+      <c r="N52" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">146, </v>
       </c>
     </row>
     <row r="53" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E53" s="24">
+      <c r="E53" s="20">
         <v>82000</v>
       </c>
       <c r="F53" s="8">
@@ -3201,16 +3201,16 @@
         <v/>
       </c>
       <c r="M53" s="7" t="str">
-        <f>IF(L53&lt;&gt;"",L53+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N53" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N53" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">178, </v>
       </c>
     </row>
     <row r="54" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E54" s="24">
+      <c r="E54" s="20">
         <v>100000</v>
       </c>
       <c r="F54" s="8">
@@ -3242,17 +3242,17 @@
         <v/>
       </c>
       <c r="M54" s="7" t="str">
-        <f>IF(L54&lt;&gt;"",L54+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N54" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N54" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">215, 
 </v>
       </c>
     </row>
     <row r="55" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E55" s="24">
+      <c r="E55" s="20">
         <v>120000</v>
       </c>
       <c r="F55" s="8">
@@ -3284,16 +3284,16 @@
         <v>50</v>
       </c>
       <c r="M55" s="7" t="str">
-        <f>IF(L55&lt;&gt;"",L55+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">68, </v>
       </c>
-      <c r="N55" s="23" t="str">
+      <c r="N55" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">132, </v>
       </c>
     </row>
     <row r="56" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E56" s="24">
+      <c r="E56" s="20">
         <v>150000</v>
       </c>
       <c r="F56" s="8">
@@ -3325,16 +3325,16 @@
         <v/>
       </c>
       <c r="M56" s="7" t="str">
-        <f>IF(L56&lt;&gt;"",L56+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N56" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N56" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">161, </v>
       </c>
     </row>
     <row r="57" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E57" s="24">
+      <c r="E57" s="20">
         <v>180000</v>
       </c>
       <c r="F57" s="8">
@@ -3366,16 +3366,16 @@
         <v/>
       </c>
       <c r="M57" s="7" t="str">
-        <f>IF(L57&lt;&gt;"",L57+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N57" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N57" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">195, </v>
       </c>
     </row>
     <row r="58" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E58" s="24">
+      <c r="E58" s="20">
         <v>220000</v>
       </c>
       <c r="F58" s="8">
@@ -3407,17 +3407,17 @@
         <v/>
       </c>
       <c r="M58" s="7" t="str">
-        <f>IF(L58&lt;&gt;"",L58+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N58" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N58" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">239, 
 </v>
       </c>
     </row>
     <row r="59" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E59" s="24">
+      <c r="E59" s="20">
         <v>270000</v>
       </c>
       <c r="F59" s="8">
@@ -3449,16 +3449,16 @@
         <v>54</v>
       </c>
       <c r="M59" s="7" t="str">
-        <f>IF(L59&lt;&gt;"",L59+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">72, </v>
       </c>
-      <c r="N59" s="23" t="str">
+      <c r="N59" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">146, </v>
       </c>
     </row>
     <row r="60" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E60" s="24">
+      <c r="E60" s="20">
         <v>330000</v>
       </c>
       <c r="F60" s="8">
@@ -3490,16 +3490,16 @@
         <v/>
       </c>
       <c r="M60" s="7" t="str">
-        <f>IF(L60&lt;&gt;"",L60+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N60" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N60" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">176, </v>
       </c>
     </row>
     <row r="61" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E61" s="24">
+      <c r="E61" s="20">
         <v>390000</v>
       </c>
       <c r="F61" s="8">
@@ -3531,16 +3531,16 @@
         <v/>
       </c>
       <c r="M61" s="7" t="str">
-        <f>IF(L61&lt;&gt;"",L61+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N61" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N61" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">210, </v>
       </c>
     </row>
     <row r="62" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E62" s="24">
+      <c r="E62" s="20">
         <v>470000</v>
       </c>
       <c r="F62" s="8">
@@ -3572,17 +3572,17 @@
         <v/>
       </c>
       <c r="M62" s="7" t="str">
-        <f>IF(L62&lt;&gt;"",L62+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N62" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N62" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">251, 
 </v>
       </c>
     </row>
     <row r="63" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E63" s="24">
+      <c r="E63" s="20">
         <v>560000</v>
       </c>
       <c r="F63" s="8">
@@ -3614,16 +3614,16 @@
         <v>58</v>
       </c>
       <c r="M63" s="7" t="str">
-        <f>IF(L63&lt;&gt;"",L63+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" ref="M63:M94" si="10">IF(L63&lt;&gt;"",L63+COUNT(L:L)&amp;", ","")</f>
         <v xml:space="preserve">76, </v>
       </c>
-      <c r="N63" s="23" t="str">
+      <c r="N63" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">151, </v>
       </c>
     </row>
     <row r="64" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E64" s="24">
+      <c r="E64" s="20">
         <v>680000</v>
       </c>
       <c r="F64" s="8">
@@ -3655,16 +3655,16 @@
         <v/>
       </c>
       <c r="M64" s="7" t="str">
-        <f>IF(L64&lt;&gt;"",L64+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N64" s="23" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="N64" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">183, </v>
       </c>
     </row>
     <row r="65" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E65" s="24">
+      <c r="E65" s="20">
         <v>820000</v>
       </c>
       <c r="F65" s="8">
@@ -3696,17 +3696,17 @@
         <v/>
       </c>
       <c r="M65" s="7" t="str">
-        <f>IF(L65&lt;&gt;"",L65+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N65" s="23" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="N65" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">222, 
 </v>
       </c>
     </row>
     <row r="66" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E66" s="24">
+      <c r="E66" s="20">
         <v>1000000</v>
       </c>
       <c r="F66" s="8">
@@ -3738,16 +3738,16 @@
         <v>61</v>
       </c>
       <c r="M66" s="7" t="str">
-        <f>IF(L66&lt;&gt;"",L66+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">79, </v>
       </c>
-      <c r="N66" s="23" t="str">
+      <c r="N66" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">134, </v>
       </c>
     </row>
     <row r="67" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E67" s="24">
+      <c r="E67" s="20">
         <v>1200000</v>
       </c>
       <c r="F67" s="8">
@@ -3779,16 +3779,16 @@
         <v/>
       </c>
       <c r="M67" s="7" t="str">
-        <f>IF(L67&lt;&gt;"",L67+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N67" s="23" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="N67" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">165, </v>
       </c>
     </row>
     <row r="68" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E68" s="24">
+      <c r="E68" s="20">
         <v>1500000</v>
       </c>
       <c r="F68" s="8">
@@ -3820,16 +3820,16 @@
         <v/>
       </c>
       <c r="M68" s="7" t="str">
-        <f>IF(L68&lt;&gt;"",L68+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N68" s="23" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="N68" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">201, </v>
       </c>
     </row>
     <row r="69" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E69" s="24">
+      <c r="E69" s="20">
         <v>1800000</v>
       </c>
       <c r="F69" s="8">
@@ -3861,398 +3861,398 @@
         <v/>
       </c>
       <c r="M69" s="7" t="str">
-        <f>IF(L69&lt;&gt;"",L69+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N69" s="23" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="N69" s="19" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">244, 
 </v>
       </c>
     </row>
     <row r="70" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E70" s="24">
+      <c r="E70" s="20">
         <v>2200000</v>
       </c>
       <c r="F70" s="8">
-        <f t="shared" ref="F70:F78" si="9">E70-(E70-E71)/2</f>
+        <f t="shared" ref="F70:F78" si="11">E70-(E70-E71)/2</f>
         <v>2450000</v>
       </c>
       <c r="G70" s="11">
-        <f t="shared" ref="G70:G78" si="10">F70/(2^$C$13)</f>
+        <f t="shared" ref="G70:G78" si="12">F70/(2^$C$13)</f>
         <v>2450000</v>
       </c>
       <c r="H70" s="6">
-        <f t="shared" ref="H70:H78" si="11">IF(CEILING(LOG(G70+1,2),1)&lt;$C$8*8,$C$8*8,CEILING(LOG(G70+1,2),1))</f>
+        <f t="shared" ref="H70:H78" si="13">IF(CEILING(LOG(G70+1,2),1)&lt;$C$8*8,$C$8*8,CEILING(LOG(G70+1,2),1))</f>
         <v>22</v>
       </c>
       <c r="I70" s="11">
-        <f t="shared" ref="I70:I78" si="12">G70/2^(H70-($C$8*8))</f>
+        <f t="shared" ref="I70:I78" si="14">G70/2^(H70-($C$8*8))</f>
         <v>149.5361328125</v>
       </c>
       <c r="J70" s="16">
-        <f t="shared" ref="J70:J78" si="13">ROUND(I70,0)</f>
+        <f t="shared" ref="J70:J78" si="15">ROUND(I70,0)</f>
         <v>150</v>
       </c>
       <c r="K70" s="17">
-        <f t="shared" ref="K70:K78" si="14">I70/J70-1</f>
+        <f t="shared" ref="K70:K78" si="16">I70/J70-1</f>
         <v>-3.0924479166666297E-3</v>
       </c>
       <c r="L70" s="6">
-        <f t="shared" ref="L70:L79" si="15">IF($H69&lt;&gt;$H70,ROW($H70)-ROW($H$5),"")</f>
+        <f t="shared" ref="L70:L79" si="17">IF($H69&lt;&gt;$H70,ROW($H70)-ROW($H$5),"")</f>
         <v>65</v>
       </c>
       <c r="M70" s="7" t="str">
-        <f>IF(L70&lt;&gt;"",L70+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">83, </v>
       </c>
-      <c r="N70" s="23" t="str">
-        <f t="shared" ref="N70:N78" si="16">IF(J70&lt;&gt;"",J70&amp;", "&amp;IF($H70&lt;&gt;$H71,CHAR(10),""),"")</f>
+      <c r="N70" s="19" t="str">
+        <f t="shared" ref="N70:N78" si="18">IF(J70&lt;&gt;"",J70&amp;", "&amp;IF($H70&lt;&gt;$H71,CHAR(10),""),"")</f>
         <v xml:space="preserve">150, </v>
       </c>
     </row>
     <row r="71" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E71" s="24">
+      <c r="E71" s="20">
         <v>2700000</v>
       </c>
       <c r="F71" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3000000</v>
       </c>
       <c r="G71" s="11">
+        <f t="shared" si="12"/>
+        <v>3000000</v>
+      </c>
+      <c r="H71" s="6">
+        <f t="shared" si="13"/>
+        <v>22</v>
+      </c>
+      <c r="I71" s="11">
+        <f t="shared" si="14"/>
+        <v>183.10546875</v>
+      </c>
+      <c r="J71" s="16">
+        <f t="shared" si="15"/>
+        <v>183</v>
+      </c>
+      <c r="K71" s="17">
+        <f t="shared" si="16"/>
+        <v>5.7633196721318392E-4</v>
+      </c>
+      <c r="L71" s="6" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="M71" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>3000000</v>
-      </c>
-      <c r="H71" s="6">
+        <v/>
+      </c>
+      <c r="N71" s="19" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">183, </v>
+      </c>
+    </row>
+    <row r="72" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E72" s="20">
+        <v>3300000</v>
+      </c>
+      <c r="F72" s="8">
         <f t="shared" si="11"/>
+        <v>3600000</v>
+      </c>
+      <c r="G72" s="11">
+        <f t="shared" si="12"/>
+        <v>3600000</v>
+      </c>
+      <c r="H72" s="6">
+        <f t="shared" si="13"/>
         <v>22</v>
       </c>
-      <c r="I71" s="11">
-        <f t="shared" si="12"/>
-        <v>183.10546875</v>
-      </c>
-      <c r="J71" s="16">
-        <f t="shared" si="13"/>
-        <v>183</v>
-      </c>
-      <c r="K71" s="17">
+      <c r="I72" s="11">
         <f t="shared" si="14"/>
-        <v>5.7633196721318392E-4</v>
-      </c>
-      <c r="L71" s="6" t="str">
+        <v>219.7265625</v>
+      </c>
+      <c r="J72" s="16">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="M71" s="7" t="str">
-        <f>IF(L71&lt;&gt;"",L71+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N71" s="23" t="str">
+        <v>220</v>
+      </c>
+      <c r="K72" s="17">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">183, </v>
-      </c>
-    </row>
-    <row r="72" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E72" s="24">
-        <v>3300000</v>
-      </c>
-      <c r="F72" s="8">
-        <f t="shared" si="9"/>
-        <v>3600000</v>
-      </c>
-      <c r="G72" s="11">
+        <v>-1.2428977272727071E-3</v>
+      </c>
+      <c r="L72" s="6" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="M72" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>3600000</v>
-      </c>
-      <c r="H72" s="6">
-        <f t="shared" si="11"/>
-        <v>22</v>
-      </c>
-      <c r="I72" s="11">
-        <f t="shared" si="12"/>
-        <v>219.7265625</v>
-      </c>
-      <c r="J72" s="16">
-        <f t="shared" si="13"/>
-        <v>220</v>
-      </c>
-      <c r="K72" s="17">
-        <f t="shared" si="14"/>
-        <v>-1.2428977272727071E-3</v>
-      </c>
-      <c r="L72" s="6" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="M72" s="7" t="str">
-        <f>IF(L72&lt;&gt;"",L72+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N72" s="23" t="str">
-        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N72" s="19" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve">220, 
 </v>
       </c>
     </row>
     <row r="73" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E73" s="24">
+      <c r="E73" s="20">
         <v>3900000</v>
       </c>
       <c r="F73" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>4300000</v>
       </c>
       <c r="G73" s="11">
+        <f t="shared" si="12"/>
+        <v>4300000</v>
+      </c>
+      <c r="H73" s="6">
+        <f t="shared" si="13"/>
+        <v>23</v>
+      </c>
+      <c r="I73" s="11">
+        <f t="shared" si="14"/>
+        <v>131.2255859375</v>
+      </c>
+      <c r="J73" s="16">
+        <f t="shared" si="15"/>
+        <v>131</v>
+      </c>
+      <c r="K73" s="17">
+        <f t="shared" si="16"/>
+        <v>1.7220300572517999E-3</v>
+      </c>
+      <c r="L73" s="6">
+        <f t="shared" si="17"/>
+        <v>68</v>
+      </c>
+      <c r="M73" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>4300000</v>
-      </c>
-      <c r="H73" s="6">
+        <v xml:space="preserve">86, </v>
+      </c>
+      <c r="N73" s="19" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">131, </v>
+      </c>
+    </row>
+    <row r="74" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E74" s="20">
+        <v>4700000</v>
+      </c>
+      <c r="F74" s="8">
         <f t="shared" si="11"/>
+        <v>5150000</v>
+      </c>
+      <c r="G74" s="11">
+        <f t="shared" si="12"/>
+        <v>5150000</v>
+      </c>
+      <c r="H74" s="6">
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
-      <c r="I73" s="11">
+      <c r="I74" s="11">
+        <f t="shared" si="14"/>
+        <v>157.16552734375</v>
+      </c>
+      <c r="J74" s="16">
+        <f t="shared" si="15"/>
+        <v>157</v>
+      </c>
+      <c r="K74" s="17">
+        <f t="shared" si="16"/>
+        <v>1.0543142914012371E-3</v>
+      </c>
+      <c r="L74" s="6" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="M74" s="7" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="N74" s="19" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">157, </v>
+      </c>
+    </row>
+    <row r="75" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E75" s="20">
+        <v>5600000</v>
+      </c>
+      <c r="F75" s="8">
+        <f t="shared" si="11"/>
+        <v>6200000</v>
+      </c>
+      <c r="G75" s="11">
         <f t="shared" si="12"/>
-        <v>131.2255859375</v>
-      </c>
-      <c r="J73" s="16">
+        <v>6200000</v>
+      </c>
+      <c r="H75" s="6">
         <f t="shared" si="13"/>
-        <v>131</v>
-      </c>
-      <c r="K73" s="17">
+        <v>23</v>
+      </c>
+      <c r="I75" s="11">
         <f t="shared" si="14"/>
-        <v>1.7220300572517999E-3</v>
-      </c>
-      <c r="L73" s="6">
+        <v>189.208984375</v>
+      </c>
+      <c r="J75" s="16">
         <f t="shared" si="15"/>
-        <v>68</v>
-      </c>
-      <c r="M73" s="7" t="str">
-        <f>IF(L73&lt;&gt;"",L73+COUNT(L:L)&amp;", ","")</f>
-        <v xml:space="preserve">86, </v>
-      </c>
-      <c r="N73" s="23" t="str">
+        <v>189</v>
+      </c>
+      <c r="K75" s="17">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">131, </v>
-      </c>
-    </row>
-    <row r="74" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E74" s="24">
-        <v>4700000</v>
-      </c>
-      <c r="F74" s="8">
-        <f t="shared" si="9"/>
-        <v>5150000</v>
-      </c>
-      <c r="G74" s="11">
+        <v>1.1057374338623305E-3</v>
+      </c>
+      <c r="L75" s="6" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="M75" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>5150000</v>
-      </c>
-      <c r="H74" s="6">
+        <v/>
+      </c>
+      <c r="N75" s="19" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">189, </v>
+      </c>
+    </row>
+    <row r="76" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E76" s="20">
+        <v>6800000</v>
+      </c>
+      <c r="F76" s="8">
         <f t="shared" si="11"/>
+        <v>7500000</v>
+      </c>
+      <c r="G76" s="11">
+        <f t="shared" si="12"/>
+        <v>7500000</v>
+      </c>
+      <c r="H76" s="6">
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
-      <c r="I74" s="11">
-        <f t="shared" si="12"/>
-        <v>157.16552734375</v>
-      </c>
-      <c r="J74" s="16">
-        <f t="shared" si="13"/>
-        <v>157</v>
-      </c>
-      <c r="K74" s="17">
+      <c r="I76" s="11">
         <f t="shared" si="14"/>
-        <v>1.0543142914012371E-3</v>
-      </c>
-      <c r="L74" s="6" t="str">
+        <v>228.8818359375</v>
+      </c>
+      <c r="J76" s="16">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="M74" s="7" t="str">
-        <f>IF(L74&lt;&gt;"",L74+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N74" s="23" t="str">
+        <v>229</v>
+      </c>
+      <c r="K76" s="17">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">157, </v>
-      </c>
-    </row>
-    <row r="75" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E75" s="24">
-        <v>5600000</v>
-      </c>
-      <c r="F75" s="8">
-        <f t="shared" si="9"/>
-        <v>6200000</v>
-      </c>
-      <c r="G75" s="11">
+        <v>-5.1600027292575401E-4</v>
+      </c>
+      <c r="L76" s="6" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="M76" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>6200000</v>
-      </c>
-      <c r="H75" s="6">
-        <f t="shared" si="11"/>
-        <v>23</v>
-      </c>
-      <c r="I75" s="11">
-        <f t="shared" si="12"/>
-        <v>189.208984375</v>
-      </c>
-      <c r="J75" s="16">
-        <f t="shared" si="13"/>
-        <v>189</v>
-      </c>
-      <c r="K75" s="17">
-        <f t="shared" si="14"/>
-        <v>1.1057374338623305E-3</v>
-      </c>
-      <c r="L75" s="6" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="M75" s="7" t="str">
-        <f>IF(L75&lt;&gt;"",L75+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N75" s="23" t="str">
-        <f t="shared" si="16"/>
-        <v xml:space="preserve">189, </v>
-      </c>
-    </row>
-    <row r="76" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E76" s="24">
-        <v>6800000</v>
-      </c>
-      <c r="F76" s="8">
-        <f t="shared" si="9"/>
-        <v>7500000</v>
-      </c>
-      <c r="G76" s="11">
-        <f t="shared" si="10"/>
-        <v>7500000</v>
-      </c>
-      <c r="H76" s="6">
-        <f t="shared" si="11"/>
-        <v>23</v>
-      </c>
-      <c r="I76" s="11">
-        <f t="shared" si="12"/>
-        <v>228.8818359375</v>
-      </c>
-      <c r="J76" s="16">
-        <f t="shared" si="13"/>
-        <v>229</v>
-      </c>
-      <c r="K76" s="17">
-        <f t="shared" si="14"/>
-        <v>-5.1600027292575401E-4</v>
-      </c>
-      <c r="L76" s="6" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="M76" s="7" t="str">
-        <f>IF(L76&lt;&gt;"",L76+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N76" s="23" t="str">
-        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N76" s="19" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve">229, 
 </v>
       </c>
     </row>
     <row r="77" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E77" s="24">
+      <c r="E77" s="20">
         <v>8200000</v>
       </c>
       <c r="F77" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>9100000</v>
       </c>
       <c r="G77" s="11">
+        <f t="shared" si="12"/>
+        <v>9100000</v>
+      </c>
+      <c r="H77" s="6">
+        <f t="shared" si="13"/>
+        <v>24</v>
+      </c>
+      <c r="I77" s="11">
+        <f t="shared" si="14"/>
+        <v>138.85498046875</v>
+      </c>
+      <c r="J77" s="16">
+        <f t="shared" si="15"/>
+        <v>139</v>
+      </c>
+      <c r="K77" s="17">
+        <f t="shared" si="16"/>
+        <v>-1.0433059802158473E-3</v>
+      </c>
+      <c r="L77" s="6">
+        <f t="shared" si="17"/>
+        <v>72</v>
+      </c>
+      <c r="M77" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>9100000</v>
-      </c>
-      <c r="H77" s="6">
+        <v xml:space="preserve">90, </v>
+      </c>
+      <c r="N77" s="19" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">139, </v>
+      </c>
+    </row>
+    <row r="78" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E78" s="20">
+        <v>10000000</v>
+      </c>
+      <c r="F78" s="8">
         <f t="shared" si="11"/>
+        <v>11000000</v>
+      </c>
+      <c r="G78" s="11">
+        <f t="shared" si="12"/>
+        <v>11000000</v>
+      </c>
+      <c r="H78" s="6">
+        <f t="shared" si="13"/>
         <v>24</v>
       </c>
-      <c r="I77" s="11">
-        <f t="shared" si="12"/>
-        <v>138.85498046875</v>
-      </c>
-      <c r="J77" s="16">
-        <f t="shared" si="13"/>
-        <v>139</v>
-      </c>
-      <c r="K77" s="17">
+      <c r="I78" s="11">
         <f t="shared" si="14"/>
-        <v>-1.0433059802158473E-3</v>
-      </c>
-      <c r="L77" s="6">
+        <v>167.8466796875</v>
+      </c>
+      <c r="J78" s="16">
         <f t="shared" si="15"/>
-        <v>72</v>
-      </c>
-      <c r="M77" s="7" t="str">
-        <f>IF(L77&lt;&gt;"",L77+COUNT(L:L)&amp;", ","")</f>
-        <v xml:space="preserve">90, </v>
-      </c>
-      <c r="N77" s="23" t="str">
+        <v>168</v>
+      </c>
+      <c r="K78" s="17">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">139, </v>
-      </c>
-    </row>
-    <row r="78" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E78" s="24">
-        <v>10000000</v>
-      </c>
-      <c r="F78" s="8">
-        <f t="shared" si="9"/>
-        <v>11000000</v>
-      </c>
-      <c r="G78" s="11">
+        <v>-9.1262090773813753E-4</v>
+      </c>
+      <c r="L78" s="6" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="M78" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>11000000</v>
-      </c>
-      <c r="H78" s="6">
-        <f t="shared" si="11"/>
-        <v>24</v>
-      </c>
-      <c r="I78" s="11">
-        <f t="shared" si="12"/>
-        <v>167.8466796875</v>
-      </c>
-      <c r="J78" s="16">
-        <f t="shared" si="13"/>
-        <v>168</v>
-      </c>
-      <c r="K78" s="17">
-        <f t="shared" si="14"/>
-        <v>-9.1262090773813753E-4</v>
-      </c>
-      <c r="L78" s="6" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="M78" s="7" t="str">
-        <f>IF(L78&lt;&gt;"",L78+COUNT(L:L)&amp;", ","")</f>
-        <v/>
-      </c>
-      <c r="N78" s="23" t="str">
-        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="N78" s="19" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve">168, 
 </v>
       </c>
     </row>
     <row r="79" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E79" s="24">
+      <c r="E79" s="20">
         <v>12000000</v>
       </c>
       <c r="H79" s="6"/>
       <c r="L79" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>74</v>
       </c>
       <c r="M79" s="7" t="str">
-        <f>IF(L79&lt;&gt;"",L79+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">92, </v>
       </c>
     </row>
@@ -4273,14 +4273,14 @@
     <sortCondition ref="E5"/>
   </sortState>
   <mergeCells count="8">
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="P5:P43"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="L3:P3"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="P5:P43"/>
-    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix results for row count <9
</commit_message>
<xml_diff>
--- a/lut_generator_E12_10R10M.xlsx
+++ b/lut_generator_E12_10R10M.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\shared\Dokumente\codebase\avr-quantizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6476FE-1160-465C-8094-978B2BC42CAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC6E741-DE0F-42D9-A4E7-202FA0E72B2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6830" yWindow="0" windowWidth="36500" windowHeight="18320" xr2:uid="{F31E432E-1247-4F18-8B99-AC2EE1672703}"/>
+    <workbookView xWindow="7810" yWindow="0" windowWidth="36500" windowHeight="18320" xr2:uid="{F31E432E-1247-4F18-8B99-AC2EE1672703}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -459,16 +459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -479,6 +470,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="5" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52672B51-097A-4F0D-94C8-36FB4DE8AA5D}">
   <dimension ref="A1:R83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" topLeftCell="D58" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5:N79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -829,29 +829,29 @@
     <row r="2" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="24"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="10"/>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="22" t="s">
+      <c r="F3" s="27"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="22" t="s">
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
     </row>
     <row r="4" spans="1:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10"/>
@@ -940,11 +940,11 @@
         <v xml:space="preserve">18, </v>
       </c>
       <c r="N5" s="19" t="str">
-        <f>IF(J5&lt;&gt;"",J5&amp;", "&amp;IF($H5&lt;&gt;$H6,CHAR(10),""),"")</f>
+        <f>IF(J5&lt;&gt;"",J5&amp;", "&amp;IF($H5&lt;&gt;$H6,CHAR(10),""),256^$C$8-1&amp;CHAR(10))</f>
         <v xml:space="preserve">9, </v>
       </c>
       <c r="O5" s="19"/>
-      <c r="P5" s="26" t="str">
+      <c r="P5" s="23" t="str">
         <f>"const __flash uint"&amp;$C$8*8&amp;"_t "&amp;"lut"&amp;$C$8&amp;"d"&amp;$C$7&amp;"_"&amp;$C$6&amp;"["&amp;COUNT($J:$J)+COUNT($L:$L)&amp;"] ="&amp;CHAR(10)&amp;"{"&amp;CHAR(10)&amp;_xlfn.CONCAT($M:$M)&amp;CHAR(10)&amp;CHAR(10)&amp;_xlfn.CONCAT($N:$N)&amp;"};"</f>
         <v>const __flash uint8_t lut1d4_E12_10R10M[92] =
 {
@@ -968,6 +968,7 @@
 150, 183, 220, 
 131, 157, 189, 229, 
 139, 168, 
+255
 };</v>
       </c>
     </row>
@@ -1016,11 +1017,11 @@
         <v/>
       </c>
       <c r="N6" s="19" t="str">
-        <f>IF(J6&lt;&gt;"",J6&amp;", "&amp;IF($H6&lt;&gt;$H7,CHAR(10),""),"")</f>
+        <f t="shared" ref="N6:N69" si="6">IF(J6&lt;&gt;"",J6&amp;", "&amp;IF($H6&lt;&gt;$H7,CHAR(10),""),256^$C$8-1&amp;CHAR(10))</f>
         <v xml:space="preserve">11, </v>
       </c>
       <c r="O6" s="19"/>
-      <c r="P6" s="27"/>
+      <c r="P6" s="24"/>
     </row>
     <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
@@ -1035,7 +1036,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="8">
-        <f t="shared" ref="F7:F69" si="6">E7-(E7-E8)/2</f>
+        <f t="shared" ref="F7:F69" si="7">E7-(E7-E8)/2</f>
         <v>13.5</v>
       </c>
       <c r="G7" s="11">
@@ -1063,15 +1064,15 @@
         <v/>
       </c>
       <c r="M7" s="7" t="str">
-        <f t="shared" ref="M7:M30" si="7">IF(L7&lt;&gt;"",L7+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" ref="M7:M30" si="8">IF(L7&lt;&gt;"",L7+COUNT(L:L)&amp;", ","")</f>
         <v/>
       </c>
       <c r="N7" s="19" t="str">
-        <f t="shared" ref="N7:N69" si="8">IF(J7&lt;&gt;"",J7&amp;", "&amp;IF($H7&lt;&gt;$H8,CHAR(10),""),"")</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">14, </v>
       </c>
       <c r="O7" s="19"/>
-      <c r="P7" s="27"/>
+      <c r="P7" s="24"/>
     </row>
     <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
@@ -1086,7 +1087,7 @@
         <v>15</v>
       </c>
       <c r="F8" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16.5</v>
       </c>
       <c r="G8" s="11">
@@ -1114,15 +1115,15 @@
         <v/>
       </c>
       <c r="M8" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N8" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">17, </v>
       </c>
       <c r="O8" s="19"/>
-      <c r="P8" s="27"/>
+      <c r="P8" s="24"/>
     </row>
     <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
@@ -1137,7 +1138,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="G9" s="11">
@@ -1165,15 +1166,15 @@
         <v/>
       </c>
       <c r="M9" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N9" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">20, </v>
       </c>
       <c r="O9" s="19"/>
-      <c r="P9" s="27"/>
+      <c r="P9" s="24"/>
     </row>
     <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
@@ -1184,7 +1185,7 @@
         <v>22</v>
       </c>
       <c r="F10" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24.5</v>
       </c>
       <c r="G10" s="11">
@@ -1212,15 +1213,15 @@
         <v/>
       </c>
       <c r="M10" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N10" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">25, </v>
       </c>
       <c r="O10" s="19"/>
-      <c r="P10" s="27"/>
+      <c r="P10" s="24"/>
     </row>
     <row r="11" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
@@ -1231,7 +1232,7 @@
         <v>27</v>
       </c>
       <c r="F11" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="G11" s="11">
@@ -1259,28 +1260,28 @@
         <v/>
       </c>
       <c r="M11" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N11" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">30, </v>
       </c>
       <c r="O11" s="19"/>
-      <c r="P11" s="27"/>
+      <c r="P11" s="24"/>
     </row>
     <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="24"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="7"/>
       <c r="E12" s="20">
         <v>33</v>
       </c>
       <c r="F12" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="G12" s="11">
@@ -1308,15 +1309,15 @@
         <v/>
       </c>
       <c r="M12" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N12" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">36, </v>
       </c>
       <c r="O12" s="19"/>
-      <c r="P12" s="27"/>
+      <c r="P12" s="24"/>
     </row>
     <row r="13" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
@@ -1332,7 +1333,7 @@
         <v>39</v>
       </c>
       <c r="F13" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43</v>
       </c>
       <c r="G13" s="11">
@@ -1360,15 +1361,15 @@
         <v/>
       </c>
       <c r="M13" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N13" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">43, </v>
       </c>
       <c r="O13" s="19"/>
-      <c r="P13" s="27"/>
+      <c r="P13" s="24"/>
     </row>
     <row r="14" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7"/>
@@ -1379,7 +1380,7 @@
         <v>47</v>
       </c>
       <c r="F14" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>51.5</v>
       </c>
       <c r="G14" s="11">
@@ -1407,28 +1408,28 @@
         <v/>
       </c>
       <c r="M14" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N14" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">52, </v>
       </c>
       <c r="O14" s="19"/>
-      <c r="P14" s="27"/>
+      <c r="P14" s="24"/>
     </row>
     <row r="15" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="24"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="7"/>
       <c r="E15" s="20">
         <v>56</v>
       </c>
       <c r="F15" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>62</v>
       </c>
       <c r="G15" s="11">
@@ -1456,19 +1457,19 @@
         <v/>
       </c>
       <c r="M15" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N15" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">62, </v>
       </c>
       <c r="O15" s="19"/>
-      <c r="P15" s="27"/>
+      <c r="P15" s="24"/>
     </row>
     <row r="16" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
-      <c r="B16" s="28" t="str">
+      <c r="B16" s="25" t="str">
         <f>$P$5</f>
         <v>const __flash uint8_t lut1d4_E12_10R10M[92] =
 {
@@ -1492,15 +1493,16 @@
 150, 183, 220, 
 131, 157, 189, 229, 
 139, 168, 
+255
 };</v>
       </c>
-      <c r="C16" s="28"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="7"/>
       <c r="E16" s="20">
         <v>68</v>
       </c>
       <c r="F16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>75</v>
       </c>
       <c r="G16" s="11">
@@ -1528,15 +1530,15 @@
         <v/>
       </c>
       <c r="M16" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N16" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">75, </v>
       </c>
       <c r="O16" s="19"/>
-      <c r="P16" s="27"/>
+      <c r="P16" s="24"/>
     </row>
     <row r="17" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
@@ -1547,7 +1549,7 @@
         <v>82</v>
       </c>
       <c r="F17" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>91</v>
       </c>
       <c r="G17" s="11">
@@ -1575,15 +1577,15 @@
         <v/>
       </c>
       <c r="M17" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N17" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">91, </v>
       </c>
       <c r="O17" s="19"/>
-      <c r="P17" s="27"/>
+      <c r="P17" s="24"/>
     </row>
     <row r="18" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7"/>
@@ -1594,7 +1596,7 @@
         <v>100</v>
       </c>
       <c r="F18" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>110</v>
       </c>
       <c r="G18" s="11">
@@ -1622,15 +1624,15 @@
         <v/>
       </c>
       <c r="M18" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N18" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">110, </v>
       </c>
       <c r="O18" s="19"/>
-      <c r="P18" s="27"/>
+      <c r="P18" s="24"/>
     </row>
     <row r="19" spans="1:16" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7"/>
@@ -1641,7 +1643,7 @@
         <v>120</v>
       </c>
       <c r="F19" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>135</v>
       </c>
       <c r="G19" s="11">
@@ -1669,15 +1671,15 @@
         <v/>
       </c>
       <c r="M19" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N19" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">135, </v>
       </c>
       <c r="O19" s="19"/>
-      <c r="P19" s="27"/>
+      <c r="P19" s="24"/>
     </row>
     <row r="20" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
@@ -1688,7 +1690,7 @@
         <v>150</v>
       </c>
       <c r="F20" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>165</v>
       </c>
       <c r="G20" s="11">
@@ -1716,15 +1718,15 @@
         <v/>
       </c>
       <c r="M20" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N20" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">165, </v>
       </c>
       <c r="O20" s="19"/>
-      <c r="P20" s="27"/>
+      <c r="P20" s="24"/>
     </row>
     <row r="21" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7"/>
@@ -1735,7 +1737,7 @@
         <v>180</v>
       </c>
       <c r="F21" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>200</v>
       </c>
       <c r="G21" s="11">
@@ -1763,15 +1765,15 @@
         <v/>
       </c>
       <c r="M21" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N21" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">200, </v>
       </c>
       <c r="O21" s="19"/>
-      <c r="P21" s="27"/>
+      <c r="P21" s="24"/>
     </row>
     <row r="22" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7"/>
@@ -1782,7 +1784,7 @@
         <v>220</v>
       </c>
       <c r="F22" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>245</v>
       </c>
       <c r="G22" s="11">
@@ -1810,16 +1812,16 @@
         <v/>
       </c>
       <c r="M22" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N22" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">245, 
 </v>
       </c>
       <c r="O22" s="19"/>
-      <c r="P22" s="27"/>
+      <c r="P22" s="24"/>
     </row>
     <row r="23" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7"/>
@@ -1830,7 +1832,7 @@
         <v>270</v>
       </c>
       <c r="F23" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>300</v>
       </c>
       <c r="G23" s="11">
@@ -1858,15 +1860,15 @@
         <v>18</v>
       </c>
       <c r="M23" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">36, </v>
       </c>
       <c r="N23" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">150, </v>
       </c>
       <c r="O23" s="19"/>
-      <c r="P23" s="27"/>
+      <c r="P23" s="24"/>
     </row>
     <row r="24" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7"/>
@@ -1877,7 +1879,7 @@
         <v>330</v>
       </c>
       <c r="F24" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>360</v>
       </c>
       <c r="G24" s="11">
@@ -1905,15 +1907,15 @@
         <v/>
       </c>
       <c r="M24" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N24" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">180, </v>
       </c>
       <c r="O24" s="19"/>
-      <c r="P24" s="27"/>
+      <c r="P24" s="24"/>
     </row>
     <row r="25" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7"/>
@@ -1924,7 +1926,7 @@
         <v>390</v>
       </c>
       <c r="F25" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>430</v>
       </c>
       <c r="G25" s="11">
@@ -1952,16 +1954,16 @@
         <v/>
       </c>
       <c r="M25" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N25" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">215, 
 </v>
       </c>
       <c r="O25" s="19"/>
-      <c r="P25" s="27"/>
+      <c r="P25" s="24"/>
     </row>
     <row r="26" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7"/>
@@ -1972,7 +1974,7 @@
         <v>470</v>
       </c>
       <c r="F26" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>515</v>
       </c>
       <c r="G26" s="11">
@@ -2000,15 +2002,15 @@
         <v>21</v>
       </c>
       <c r="M26" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">39, </v>
       </c>
       <c r="N26" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">129, </v>
       </c>
       <c r="O26" s="19"/>
-      <c r="P26" s="27"/>
+      <c r="P26" s="24"/>
     </row>
     <row r="27" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7"/>
@@ -2019,7 +2021,7 @@
         <v>560</v>
       </c>
       <c r="F27" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>620</v>
       </c>
       <c r="G27" s="11">
@@ -2047,15 +2049,15 @@
         <v/>
       </c>
       <c r="M27" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N27" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">155, </v>
       </c>
       <c r="O27" s="19"/>
-      <c r="P27" s="27"/>
+      <c r="P27" s="24"/>
     </row>
     <row r="28" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7"/>
@@ -2066,7 +2068,7 @@
         <v>680</v>
       </c>
       <c r="F28" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>750</v>
       </c>
       <c r="G28" s="11">
@@ -2094,15 +2096,15 @@
         <v/>
       </c>
       <c r="M28" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N28" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">188, </v>
       </c>
       <c r="O28" s="19"/>
-      <c r="P28" s="27"/>
+      <c r="P28" s="24"/>
     </row>
     <row r="29" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="7"/>
@@ -2113,7 +2115,7 @@
         <v>820</v>
       </c>
       <c r="F29" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>910</v>
       </c>
       <c r="G29" s="11">
@@ -2141,16 +2143,16 @@
         <v/>
       </c>
       <c r="M29" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="N29" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">228, 
 </v>
       </c>
       <c r="O29" s="19"/>
-      <c r="P29" s="27"/>
+      <c r="P29" s="24"/>
     </row>
     <row r="30" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7"/>
@@ -2161,7 +2163,7 @@
         <v>1000</v>
       </c>
       <c r="F30" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1100</v>
       </c>
       <c r="G30" s="11">
@@ -2189,15 +2191,15 @@
         <v>25</v>
       </c>
       <c r="M30" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">43, </v>
       </c>
       <c r="N30" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">138, </v>
       </c>
       <c r="O30" s="19"/>
-      <c r="P30" s="27"/>
+      <c r="P30" s="24"/>
     </row>
     <row r="31" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="7"/>
@@ -2208,7 +2210,7 @@
         <v>1200</v>
       </c>
       <c r="F31" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1350</v>
       </c>
       <c r="G31" s="11">
@@ -2240,11 +2242,11 @@
         <v/>
       </c>
       <c r="N31" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">169, </v>
       </c>
       <c r="O31" s="19"/>
-      <c r="P31" s="27"/>
+      <c r="P31" s="24"/>
     </row>
     <row r="32" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7"/>
@@ -2255,7 +2257,7 @@
         <v>1500</v>
       </c>
       <c r="F32" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1650</v>
       </c>
       <c r="G32" s="11">
@@ -2287,11 +2289,11 @@
         <v/>
       </c>
       <c r="N32" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">206, </v>
       </c>
       <c r="O32" s="19"/>
-      <c r="P32" s="27"/>
+      <c r="P32" s="24"/>
     </row>
     <row r="33" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7"/>
@@ -2302,7 +2304,7 @@
         <v>1800</v>
       </c>
       <c r="F33" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2000</v>
       </c>
       <c r="G33" s="11">
@@ -2334,12 +2336,12 @@
         <v/>
       </c>
       <c r="N33" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">250, 
 </v>
       </c>
       <c r="O33" s="19"/>
-      <c r="P33" s="27"/>
+      <c r="P33" s="24"/>
       <c r="R33" s="21"/>
     </row>
     <row r="34" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2351,7 +2353,7 @@
         <v>2200</v>
       </c>
       <c r="F34" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2450</v>
       </c>
       <c r="G34" s="11">
@@ -2383,11 +2385,11 @@
         <v xml:space="preserve">47, </v>
       </c>
       <c r="N34" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">153, </v>
       </c>
       <c r="O34" s="19"/>
-      <c r="P34" s="27"/>
+      <c r="P34" s="24"/>
     </row>
     <row r="35" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6"/>
@@ -2398,7 +2400,7 @@
         <v>2700</v>
       </c>
       <c r="F35" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3000</v>
       </c>
       <c r="G35" s="11">
@@ -2430,11 +2432,11 @@
         <v/>
       </c>
       <c r="N35" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">188, </v>
       </c>
       <c r="O35" s="19"/>
-      <c r="P35" s="27"/>
+      <c r="P35" s="24"/>
     </row>
     <row r="36" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
@@ -2445,7 +2447,7 @@
         <v>3300</v>
       </c>
       <c r="F36" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3600</v>
       </c>
       <c r="G36" s="11">
@@ -2477,12 +2479,12 @@
         <v/>
       </c>
       <c r="N36" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">225, 
 </v>
       </c>
       <c r="O36" s="19"/>
-      <c r="P36" s="27"/>
+      <c r="P36" s="24"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B37" s="3"/>
@@ -2491,7 +2493,7 @@
         <v>3900</v>
       </c>
       <c r="F37" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4300</v>
       </c>
       <c r="G37" s="11">
@@ -2523,11 +2525,11 @@
         <v xml:space="preserve">50, </v>
       </c>
       <c r="N37" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">134, </v>
       </c>
       <c r="O37" s="19"/>
-      <c r="P37" s="27"/>
+      <c r="P37" s="24"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B38" s="3"/>
@@ -2536,7 +2538,7 @@
         <v>4700</v>
       </c>
       <c r="F38" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5150</v>
       </c>
       <c r="G38" s="11">
@@ -2568,11 +2570,11 @@
         <v/>
       </c>
       <c r="N38" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">161, </v>
       </c>
       <c r="O38" s="19"/>
-      <c r="P38" s="27"/>
+      <c r="P38" s="24"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B39" s="3"/>
@@ -2581,7 +2583,7 @@
         <v>5600</v>
       </c>
       <c r="F39" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6200</v>
       </c>
       <c r="G39" s="11">
@@ -2613,11 +2615,11 @@
         <v/>
       </c>
       <c r="N39" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">194, </v>
       </c>
       <c r="O39" s="19"/>
-      <c r="P39" s="27"/>
+      <c r="P39" s="24"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C40" s="7"/>
@@ -2625,7 +2627,7 @@
         <v>6800</v>
       </c>
       <c r="F40" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7500</v>
       </c>
       <c r="G40" s="11">
@@ -2657,19 +2659,19 @@
         <v/>
       </c>
       <c r="N40" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">234, 
 </v>
       </c>
       <c r="O40" s="19"/>
-      <c r="P40" s="27"/>
+      <c r="P40" s="24"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E41" s="20">
         <v>8200</v>
       </c>
       <c r="F41" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9100</v>
       </c>
       <c r="G41" s="11">
@@ -2701,18 +2703,18 @@
         <v xml:space="preserve">54, </v>
       </c>
       <c r="N41" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">142, </v>
       </c>
       <c r="O41" s="19"/>
-      <c r="P41" s="27"/>
+      <c r="P41" s="24"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E42" s="20">
         <v>10000</v>
       </c>
       <c r="F42" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11000</v>
       </c>
       <c r="G42" s="11">
@@ -2744,18 +2746,18 @@
         <v/>
       </c>
       <c r="N42" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">172, </v>
       </c>
       <c r="O42" s="19"/>
-      <c r="P42" s="27"/>
+      <c r="P42" s="24"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E43" s="20">
         <v>12000</v>
       </c>
       <c r="F43" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13500</v>
       </c>
       <c r="G43" s="11">
@@ -2787,19 +2789,19 @@
         <v/>
       </c>
       <c r="N43" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">211, 
 </v>
       </c>
       <c r="O43" s="19"/>
-      <c r="P43" s="27"/>
+      <c r="P43" s="24"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E44" s="20">
         <v>15000</v>
       </c>
       <c r="F44" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16500</v>
       </c>
       <c r="G44" s="11">
@@ -2831,7 +2833,7 @@
         <v xml:space="preserve">57, </v>
       </c>
       <c r="N44" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">129, </v>
       </c>
       <c r="O44" s="6"/>
@@ -2841,7 +2843,7 @@
         <v>18000</v>
       </c>
       <c r="F45" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>20000</v>
       </c>
       <c r="G45" s="11">
@@ -2873,7 +2875,7 @@
         <v/>
       </c>
       <c r="N45" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">156, </v>
       </c>
       <c r="O45" s="6"/>
@@ -2883,7 +2885,7 @@
         <v>22000</v>
       </c>
       <c r="F46" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24500</v>
       </c>
       <c r="G46" s="11">
@@ -2915,7 +2917,7 @@
         <v/>
       </c>
       <c r="N46" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">191, </v>
       </c>
     </row>
@@ -2924,7 +2926,7 @@
         <v>27000</v>
       </c>
       <c r="F47" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>30000</v>
       </c>
       <c r="G47" s="11">
@@ -2956,7 +2958,7 @@
         <v/>
       </c>
       <c r="N47" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">234, 
 </v>
       </c>
@@ -2966,7 +2968,7 @@
         <v>33000</v>
       </c>
       <c r="F48" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>36000</v>
       </c>
       <c r="G48" s="11">
@@ -2998,7 +3000,7 @@
         <v xml:space="preserve">61, </v>
       </c>
       <c r="N48" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">141, </v>
       </c>
       <c r="O48" s="6"/>
@@ -3008,7 +3010,7 @@
         <v>39000</v>
       </c>
       <c r="F49" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43000</v>
       </c>
       <c r="G49" s="11">
@@ -3040,7 +3042,7 @@
         <v/>
       </c>
       <c r="N49" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">168, </v>
       </c>
     </row>
@@ -3049,7 +3051,7 @@
         <v>47000</v>
       </c>
       <c r="F50" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>51500</v>
       </c>
       <c r="G50" s="11">
@@ -3081,7 +3083,7 @@
         <v/>
       </c>
       <c r="N50" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">201, </v>
       </c>
     </row>
@@ -3090,7 +3092,7 @@
         <v>56000</v>
       </c>
       <c r="F51" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>62000</v>
       </c>
       <c r="G51" s="11">
@@ -3122,7 +3124,7 @@
         <v/>
       </c>
       <c r="N51" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">242, 
 </v>
       </c>
@@ -3132,7 +3134,7 @@
         <v>68000</v>
       </c>
       <c r="F52" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>75000</v>
       </c>
       <c r="G52" s="11">
@@ -3164,7 +3166,7 @@
         <v xml:space="preserve">65, </v>
       </c>
       <c r="N52" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">146, </v>
       </c>
     </row>
@@ -3173,7 +3175,7 @@
         <v>82000</v>
       </c>
       <c r="F53" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>91000</v>
       </c>
       <c r="G53" s="11">
@@ -3205,7 +3207,7 @@
         <v/>
       </c>
       <c r="N53" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">178, </v>
       </c>
     </row>
@@ -3214,7 +3216,7 @@
         <v>100000</v>
       </c>
       <c r="F54" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>110000</v>
       </c>
       <c r="G54" s="11">
@@ -3246,7 +3248,7 @@
         <v/>
       </c>
       <c r="N54" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">215, 
 </v>
       </c>
@@ -3256,7 +3258,7 @@
         <v>120000</v>
       </c>
       <c r="F55" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>135000</v>
       </c>
       <c r="G55" s="11">
@@ -3288,7 +3290,7 @@
         <v xml:space="preserve">68, </v>
       </c>
       <c r="N55" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">132, </v>
       </c>
     </row>
@@ -3297,7 +3299,7 @@
         <v>150000</v>
       </c>
       <c r="F56" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>165000</v>
       </c>
       <c r="G56" s="11">
@@ -3329,7 +3331,7 @@
         <v/>
       </c>
       <c r="N56" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">161, </v>
       </c>
     </row>
@@ -3338,7 +3340,7 @@
         <v>180000</v>
       </c>
       <c r="F57" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>200000</v>
       </c>
       <c r="G57" s="11">
@@ -3370,7 +3372,7 @@
         <v/>
       </c>
       <c r="N57" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">195, </v>
       </c>
     </row>
@@ -3379,7 +3381,7 @@
         <v>220000</v>
       </c>
       <c r="F58" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>245000</v>
       </c>
       <c r="G58" s="11">
@@ -3411,7 +3413,7 @@
         <v/>
       </c>
       <c r="N58" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">239, 
 </v>
       </c>
@@ -3421,7 +3423,7 @@
         <v>270000</v>
       </c>
       <c r="F59" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>300000</v>
       </c>
       <c r="G59" s="11">
@@ -3453,7 +3455,7 @@
         <v xml:space="preserve">72, </v>
       </c>
       <c r="N59" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">146, </v>
       </c>
     </row>
@@ -3462,7 +3464,7 @@
         <v>330000</v>
       </c>
       <c r="F60" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>360000</v>
       </c>
       <c r="G60" s="11">
@@ -3494,7 +3496,7 @@
         <v/>
       </c>
       <c r="N60" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">176, </v>
       </c>
     </row>
@@ -3503,7 +3505,7 @@
         <v>390000</v>
       </c>
       <c r="F61" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>430000</v>
       </c>
       <c r="G61" s="11">
@@ -3535,7 +3537,7 @@
         <v/>
       </c>
       <c r="N61" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">210, </v>
       </c>
     </row>
@@ -3544,7 +3546,7 @@
         <v>470000</v>
       </c>
       <c r="F62" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>515000</v>
       </c>
       <c r="G62" s="11">
@@ -3576,7 +3578,7 @@
         <v/>
       </c>
       <c r="N62" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">251, 
 </v>
       </c>
@@ -3586,7 +3588,7 @@
         <v>560000</v>
       </c>
       <c r="F63" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>620000</v>
       </c>
       <c r="G63" s="11">
@@ -3614,11 +3616,11 @@
         <v>58</v>
       </c>
       <c r="M63" s="7" t="str">
-        <f t="shared" ref="M63:M94" si="10">IF(L63&lt;&gt;"",L63+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" ref="M63:M79" si="10">IF(L63&lt;&gt;"",L63+COUNT(L:L)&amp;", ","")</f>
         <v xml:space="preserve">76, </v>
       </c>
       <c r="N63" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">151, </v>
       </c>
     </row>
@@ -3627,7 +3629,7 @@
         <v>680000</v>
       </c>
       <c r="F64" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>750000</v>
       </c>
       <c r="G64" s="11">
@@ -3659,7 +3661,7 @@
         <v/>
       </c>
       <c r="N64" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">183, </v>
       </c>
     </row>
@@ -3668,7 +3670,7 @@
         <v>820000</v>
       </c>
       <c r="F65" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>910000</v>
       </c>
       <c r="G65" s="11">
@@ -3700,7 +3702,7 @@
         <v/>
       </c>
       <c r="N65" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">222, 
 </v>
       </c>
@@ -3710,7 +3712,7 @@
         <v>1000000</v>
       </c>
       <c r="F66" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1100000</v>
       </c>
       <c r="G66" s="11">
@@ -3742,7 +3744,7 @@
         <v xml:space="preserve">79, </v>
       </c>
       <c r="N66" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">134, </v>
       </c>
     </row>
@@ -3751,7 +3753,7 @@
         <v>1200000</v>
       </c>
       <c r="F67" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1350000</v>
       </c>
       <c r="G67" s="11">
@@ -3783,7 +3785,7 @@
         <v/>
       </c>
       <c r="N67" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">165, </v>
       </c>
     </row>
@@ -3792,7 +3794,7 @@
         <v>1500000</v>
       </c>
       <c r="F68" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1650000</v>
       </c>
       <c r="G68" s="11">
@@ -3824,7 +3826,7 @@
         <v/>
       </c>
       <c r="N68" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">201, </v>
       </c>
     </row>
@@ -3833,7 +3835,7 @@
         <v>1800000</v>
       </c>
       <c r="F69" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2000000</v>
       </c>
       <c r="G69" s="11">
@@ -3865,7 +3867,7 @@
         <v/>
       </c>
       <c r="N69" s="19" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">244, 
 </v>
       </c>
@@ -3907,7 +3909,7 @@
         <v xml:space="preserve">83, </v>
       </c>
       <c r="N70" s="19" t="str">
-        <f t="shared" ref="N70:N78" si="18">IF(J70&lt;&gt;"",J70&amp;", "&amp;IF($H70&lt;&gt;$H71,CHAR(10),""),"")</f>
+        <f t="shared" ref="N70:N79" si="18">IF(J70&lt;&gt;"",J70&amp;", "&amp;IF($H70&lt;&gt;$H71,CHAR(10),""),256^$C$8-1&amp;CHAR(10))</f>
         <v xml:space="preserve">150, </v>
       </c>
     </row>
@@ -4254,6 +4256,11 @@
       <c r="M79" s="7" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve">92, </v>
+      </c>
+      <c r="N79" s="19" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">255
+</v>
       </c>
     </row>
     <row r="80" spans="5:14" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fix LUT array size
</commit_message>
<xml_diff>
--- a/lut_generator_E12_10R10M.xlsx
+++ b/lut_generator_E12_10R10M.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\shared\Dokumente\codebase\avr-quantizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC6E741-DE0F-42D9-A4E7-202FA0E72B2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22536AAE-581B-4CA5-B295-6AB2D47398D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7810" yWindow="0" windowWidth="36500" windowHeight="18320" xr2:uid="{F31E432E-1247-4F18-8B99-AC2EE1672703}"/>
   </bookViews>
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52672B51-097A-4F0D-94C8-36FB4DE8AA5D}">
   <dimension ref="A1:R83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D58" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5:N79"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5:P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -945,8 +945,8 @@
       </c>
       <c r="O5" s="19"/>
       <c r="P5" s="23" t="str">
-        <f>"const __flash uint"&amp;$C$8*8&amp;"_t "&amp;"lut"&amp;$C$8&amp;"d"&amp;$C$7&amp;"_"&amp;$C$6&amp;"["&amp;COUNT($J:$J)+COUNT($L:$L)&amp;"] ="&amp;CHAR(10)&amp;"{"&amp;CHAR(10)&amp;_xlfn.CONCAT($M:$M)&amp;CHAR(10)&amp;CHAR(10)&amp;_xlfn.CONCAT($N:$N)&amp;"};"</f>
-        <v>const __flash uint8_t lut1d4_E12_10R10M[92] =
+        <f>"const __flash uint"&amp;$C$8*8&amp;"_t "&amp;"lut"&amp;$C$8&amp;"d"&amp;$C$7&amp;"_"&amp;$C$6&amp;"["&amp;COUNT($J:$J)+1+COUNT($L:$L)&amp;"] ="&amp;CHAR(10)&amp;"{"&amp;CHAR(10)&amp;_xlfn.CONCAT($M:$M)&amp;CHAR(10)&amp;CHAR(10)&amp;_xlfn.CONCAT($N:$N)&amp;"};"</f>
+        <v>const __flash uint8_t lut1d4_E12_10R10M[93] =
 {
 // header
 18, 36, 39, 43, 47, 50, 54, 57, 61, 65, 68, 72, 76, 79, 83, 86, 90, 92, 
@@ -1471,7 +1471,7 @@
       <c r="A16" s="7"/>
       <c r="B16" s="25" t="str">
         <f>$P$5</f>
-        <v>const __flash uint8_t lut1d4_E12_10R10M[92] =
+        <v>const __flash uint8_t lut1d4_E12_10R10M[93] =
 {
 // header
 18, 36, 39, 43, 47, 50, 54, 57, 61, 65, 68, 72, 76, 79, 83, 86, 90, 92, 

</xml_diff>

<commit_message>
Implement uint8 and uint32 variants, tests successful
</commit_message>
<xml_diff>
--- a/lut_generator_E12_10R10M.xlsx
+++ b/lut_generator_E12_10R10M.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\shared\Dokumente\codebase\avr-quantizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22536AAE-581B-4CA5-B295-6AB2D47398D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D61414-CC31-4986-BF7F-0D79C58C8133}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7810" yWindow="0" windowWidth="36500" windowHeight="18320" xr2:uid="{F31E432E-1247-4F18-8B99-AC2EE1672703}"/>
   </bookViews>
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52672B51-097A-4F0D-94C8-36FB4DE8AA5D}">
   <dimension ref="A1:R83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5:P43"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="Q67" sqref="Q67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -822,7 +822,7 @@
     <col min="12" max="12" width="11.08984375" style="6" customWidth="1"/>
     <col min="13" max="14" width="11.08984375" customWidth="1"/>
     <col min="15" max="15" width="2.81640625" customWidth="1"/>
-    <col min="16" max="16" width="40.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="59.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.45"/>
@@ -945,8 +945,8 @@
       </c>
       <c r="O5" s="19"/>
       <c r="P5" s="23" t="str">
-        <f>"const __flash uint"&amp;$C$8*8&amp;"_t "&amp;"lut"&amp;$C$8&amp;"d"&amp;$C$7&amp;"_"&amp;$C$6&amp;"["&amp;COUNT($J:$J)+1+COUNT($L:$L)&amp;"] ="&amp;CHAR(10)&amp;"{"&amp;CHAR(10)&amp;_xlfn.CONCAT($M:$M)&amp;CHAR(10)&amp;CHAR(10)&amp;_xlfn.CONCAT($N:$N)&amp;"};"</f>
-        <v>const __flash uint8_t lut1d4_E12_10R10M[93] =
+        <f>"const __flash uint"&amp;$C$8*8&amp;"_t "&amp;"lut"&amp;$C$7*8&amp;"_"&amp;$C$6&amp;"["&amp;COUNT($J:$J)+1+COUNT($L:$L)&amp;"] ="&amp;CHAR(10)&amp;"{"&amp;CHAR(10)&amp;_xlfn.CONCAT($M:$M)&amp;CHAR(10)&amp;CHAR(10)&amp;_xlfn.CONCAT($N:$N)&amp;"};"</f>
+        <v>const __flash uint8_t lut32_E12_10R10M[93] =
 {
 // header
 18, 36, 39, 43, 47, 50, 54, 57, 61, 65, 68, 72, 76, 79, 83, 86, 90, 92, 
@@ -1471,7 +1471,7 @@
       <c r="A16" s="7"/>
       <c r="B16" s="25" t="str">
         <f>$P$5</f>
-        <v>const __flash uint8_t lut1d4_E12_10R10M[93] =
+        <v>const __flash uint8_t lut32_E12_10R10M[93] =
 {
 // header
 18, 36, 39, 43, 47, 50, 54, 57, 61, 65, 68, 72, 76, 79, 83, 86, 90, 92, 

</xml_diff>

<commit_message>
Update LUTs for more precise binning boarders
See explanation in quantizer.h file
</commit_message>
<xml_diff>
--- a/lut_generator_E12_10R10M.xlsx
+++ b/lut_generator_E12_10R10M.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\shared\Dokumente\codebase\avr-quantizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D61414-CC31-4986-BF7F-0D79C58C8133}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6624AE-7DE6-43E6-871F-9674E8F72D8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7810" yWindow="0" windowWidth="36500" windowHeight="18320" xr2:uid="{F31E432E-1247-4F18-8B99-AC2EE1672703}"/>
   </bookViews>
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52672B51-097A-4F0D-94C8-36FB4DE8AA5D}">
   <dimension ref="A1:R83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="Q67" sqref="Q67"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -940,8 +940,8 @@
         <v xml:space="preserve">18, </v>
       </c>
       <c r="N5" s="19" t="str">
-        <f>IF(J5&lt;&gt;"",J5&amp;", "&amp;IF($H5&lt;&gt;$H6,CHAR(10),""),256^$C$8-1&amp;CHAR(10))</f>
-        <v xml:space="preserve">9, </v>
+        <f>IF(J5&lt;&gt;"",J5-1&amp;", "&amp;IF($H5&lt;&gt;$H6,CHAR(10),""),256^$C$8-1&amp;CHAR(10))</f>
+        <v xml:space="preserve">8, </v>
       </c>
       <c r="O5" s="19"/>
       <c r="P5" s="23" t="str">
@@ -951,23 +951,23 @@
 // header
 18, 36, 39, 43, 47, 50, 54, 57, 61, 65, 68, 72, 76, 79, 83, 86, 90, 92, 
 // data
-9, 11, 14, 17, 20, 25, 30, 36, 43, 52, 62, 75, 91, 110, 135, 165, 200, 245, 
-150, 180, 215, 
-129, 155, 188, 228, 
-138, 169, 206, 250, 
-153, 188, 225, 
-134, 161, 194, 234, 
-142, 172, 211, 
-129, 156, 191, 234, 
-141, 168, 201, 242, 
-146, 178, 215, 
-132, 161, 195, 239, 
-146, 176, 210, 251, 
-151, 183, 222, 
-134, 165, 201, 244, 
-150, 183, 220, 
-131, 157, 189, 229, 
-139, 168, 
+8, 10, 13, 16, 19, 24, 29, 35, 42, 51, 61, 74, 90, 109, 134, 164, 199, 244, 
+149, 179, 214, 
+128, 154, 187, 227, 
+137, 168, 205, 249, 
+152, 187, 224, 
+133, 160, 193, 233, 
+141, 171, 210, 
+128, 155, 190, 233, 
+140, 167, 200, 241, 
+145, 177, 214, 
+131, 160, 194, 238, 
+145, 175, 209, 250, 
+150, 182, 221, 
+133, 164, 200, 243, 
+149, 182, 219, 
+130, 156, 188, 228, 
+138, 167, 
 255
 };</v>
       </c>
@@ -1017,8 +1017,8 @@
         <v/>
       </c>
       <c r="N6" s="19" t="str">
-        <f t="shared" ref="N6:N69" si="6">IF(J6&lt;&gt;"",J6&amp;", "&amp;IF($H6&lt;&gt;$H7,CHAR(10),""),256^$C$8-1&amp;CHAR(10))</f>
-        <v xml:space="preserve">11, </v>
+        <f t="shared" ref="N6:N69" si="6">IF(J6&lt;&gt;"",J6-1&amp;", "&amp;IF($H6&lt;&gt;$H7,CHAR(10),""),256^$C$8-1&amp;CHAR(10))</f>
+        <v xml:space="preserve">10, </v>
       </c>
       <c r="O6" s="19"/>
       <c r="P6" s="24"/>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="N7" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">14, </v>
+        <v xml:space="preserve">13, </v>
       </c>
       <c r="O7" s="19"/>
       <c r="P7" s="24"/>
@@ -1120,7 +1120,7 @@
       </c>
       <c r="N8" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">17, </v>
+        <v xml:space="preserve">16, </v>
       </c>
       <c r="O8" s="19"/>
       <c r="P8" s="24"/>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="N9" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">20, </v>
+        <v xml:space="preserve">19, </v>
       </c>
       <c r="O9" s="19"/>
       <c r="P9" s="24"/>
@@ -1218,7 +1218,7 @@
       </c>
       <c r="N10" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">25, </v>
+        <v xml:space="preserve">24, </v>
       </c>
       <c r="O10" s="19"/>
       <c r="P10" s="24"/>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="N11" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">30, </v>
+        <v xml:space="preserve">29, </v>
       </c>
       <c r="O11" s="19"/>
       <c r="P11" s="24"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="N12" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">36, </v>
+        <v xml:space="preserve">35, </v>
       </c>
       <c r="O12" s="19"/>
       <c r="P12" s="24"/>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="N13" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">43, </v>
+        <v xml:space="preserve">42, </v>
       </c>
       <c r="O13" s="19"/>
       <c r="P13" s="24"/>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="N14" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">52, </v>
+        <v xml:space="preserve">51, </v>
       </c>
       <c r="O14" s="19"/>
       <c r="P14" s="24"/>
@@ -1462,7 +1462,7 @@
       </c>
       <c r="N15" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">62, </v>
+        <v xml:space="preserve">61, </v>
       </c>
       <c r="O15" s="19"/>
       <c r="P15" s="24"/>
@@ -1476,23 +1476,23 @@
 // header
 18, 36, 39, 43, 47, 50, 54, 57, 61, 65, 68, 72, 76, 79, 83, 86, 90, 92, 
 // data
-9, 11, 14, 17, 20, 25, 30, 36, 43, 52, 62, 75, 91, 110, 135, 165, 200, 245, 
-150, 180, 215, 
-129, 155, 188, 228, 
-138, 169, 206, 250, 
-153, 188, 225, 
-134, 161, 194, 234, 
-142, 172, 211, 
-129, 156, 191, 234, 
-141, 168, 201, 242, 
-146, 178, 215, 
-132, 161, 195, 239, 
-146, 176, 210, 251, 
-151, 183, 222, 
-134, 165, 201, 244, 
-150, 183, 220, 
-131, 157, 189, 229, 
-139, 168, 
+8, 10, 13, 16, 19, 24, 29, 35, 42, 51, 61, 74, 90, 109, 134, 164, 199, 244, 
+149, 179, 214, 
+128, 154, 187, 227, 
+137, 168, 205, 249, 
+152, 187, 224, 
+133, 160, 193, 233, 
+141, 171, 210, 
+128, 155, 190, 233, 
+140, 167, 200, 241, 
+145, 177, 214, 
+131, 160, 194, 238, 
+145, 175, 209, 250, 
+150, 182, 221, 
+133, 164, 200, 243, 
+149, 182, 219, 
+130, 156, 188, 228, 
+138, 167, 
 255
 };</v>
       </c>
@@ -1535,7 +1535,7 @@
       </c>
       <c r="N16" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">75, </v>
+        <v xml:space="preserve">74, </v>
       </c>
       <c r="O16" s="19"/>
       <c r="P16" s="24"/>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="N17" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">91, </v>
+        <v xml:space="preserve">90, </v>
       </c>
       <c r="O17" s="19"/>
       <c r="P17" s="24"/>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="N18" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">110, </v>
+        <v xml:space="preserve">109, </v>
       </c>
       <c r="O18" s="19"/>
       <c r="P18" s="24"/>
@@ -1676,7 +1676,7 @@
       </c>
       <c r="N19" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">135, </v>
+        <v xml:space="preserve">134, </v>
       </c>
       <c r="O19" s="19"/>
       <c r="P19" s="24"/>
@@ -1723,7 +1723,7 @@
       </c>
       <c r="N20" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">165, </v>
+        <v xml:space="preserve">164, </v>
       </c>
       <c r="O20" s="19"/>
       <c r="P20" s="24"/>
@@ -1770,7 +1770,7 @@
       </c>
       <c r="N21" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">200, </v>
+        <v xml:space="preserve">199, </v>
       </c>
       <c r="O21" s="19"/>
       <c r="P21" s="24"/>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="N22" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">245, 
+        <v xml:space="preserve">244, 
 </v>
       </c>
       <c r="O22" s="19"/>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="N23" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">150, </v>
+        <v xml:space="preserve">149, </v>
       </c>
       <c r="O23" s="19"/>
       <c r="P23" s="24"/>
@@ -1912,7 +1912,7 @@
       </c>
       <c r="N24" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">180, </v>
+        <v xml:space="preserve">179, </v>
       </c>
       <c r="O24" s="19"/>
       <c r="P24" s="24"/>
@@ -1959,7 +1959,7 @@
       </c>
       <c r="N25" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">215, 
+        <v xml:space="preserve">214, 
 </v>
       </c>
       <c r="O25" s="19"/>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="N26" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">129, </v>
+        <v xml:space="preserve">128, </v>
       </c>
       <c r="O26" s="19"/>
       <c r="P26" s="24"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="N27" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">155, </v>
+        <v xml:space="preserve">154, </v>
       </c>
       <c r="O27" s="19"/>
       <c r="P27" s="24"/>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="N28" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">188, </v>
+        <v xml:space="preserve">187, </v>
       </c>
       <c r="O28" s="19"/>
       <c r="P28" s="24"/>
@@ -2148,7 +2148,7 @@
       </c>
       <c r="N29" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">228, 
+        <v xml:space="preserve">227, 
 </v>
       </c>
       <c r="O29" s="19"/>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="N30" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">138, </v>
+        <v xml:space="preserve">137, </v>
       </c>
       <c r="O30" s="19"/>
       <c r="P30" s="24"/>
@@ -2243,7 +2243,7 @@
       </c>
       <c r="N31" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">169, </v>
+        <v xml:space="preserve">168, </v>
       </c>
       <c r="O31" s="19"/>
       <c r="P31" s="24"/>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="N32" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">206, </v>
+        <v xml:space="preserve">205, </v>
       </c>
       <c r="O32" s="19"/>
       <c r="P32" s="24"/>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="N33" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">250, 
+        <v xml:space="preserve">249, 
 </v>
       </c>
       <c r="O33" s="19"/>
@@ -2386,7 +2386,7 @@
       </c>
       <c r="N34" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">153, </v>
+        <v xml:space="preserve">152, </v>
       </c>
       <c r="O34" s="19"/>
       <c r="P34" s="24"/>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="N35" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">188, </v>
+        <v xml:space="preserve">187, </v>
       </c>
       <c r="O35" s="19"/>
       <c r="P35" s="24"/>
@@ -2480,7 +2480,7 @@
       </c>
       <c r="N36" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">225, 
+        <v xml:space="preserve">224, 
 </v>
       </c>
       <c r="O36" s="19"/>
@@ -2526,7 +2526,7 @@
       </c>
       <c r="N37" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">134, </v>
+        <v xml:space="preserve">133, </v>
       </c>
       <c r="O37" s="19"/>
       <c r="P37" s="24"/>
@@ -2571,7 +2571,7 @@
       </c>
       <c r="N38" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">161, </v>
+        <v xml:space="preserve">160, </v>
       </c>
       <c r="O38" s="19"/>
       <c r="P38" s="24"/>
@@ -2616,7 +2616,7 @@
       </c>
       <c r="N39" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">194, </v>
+        <v xml:space="preserve">193, </v>
       </c>
       <c r="O39" s="19"/>
       <c r="P39" s="24"/>
@@ -2660,7 +2660,7 @@
       </c>
       <c r="N40" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">234, 
+        <v xml:space="preserve">233, 
 </v>
       </c>
       <c r="O40" s="19"/>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="N41" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">142, </v>
+        <v xml:space="preserve">141, </v>
       </c>
       <c r="O41" s="19"/>
       <c r="P41" s="24"/>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="N42" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">172, </v>
+        <v xml:space="preserve">171, </v>
       </c>
       <c r="O42" s="19"/>
       <c r="P42" s="24"/>
@@ -2790,7 +2790,7 @@
       </c>
       <c r="N43" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">211, 
+        <v xml:space="preserve">210, 
 </v>
       </c>
       <c r="O43" s="19"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="N44" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">129, </v>
+        <v xml:space="preserve">128, </v>
       </c>
       <c r="O44" s="6"/>
     </row>
@@ -2876,7 +2876,7 @@
       </c>
       <c r="N45" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">156, </v>
+        <v xml:space="preserve">155, </v>
       </c>
       <c r="O45" s="6"/>
     </row>
@@ -2918,7 +2918,7 @@
       </c>
       <c r="N46" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">191, </v>
+        <v xml:space="preserve">190, </v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.35">
@@ -2959,7 +2959,7 @@
       </c>
       <c r="N47" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">234, 
+        <v xml:space="preserve">233, 
 </v>
       </c>
     </row>
@@ -3001,7 +3001,7 @@
       </c>
       <c r="N48" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">141, </v>
+        <v xml:space="preserve">140, </v>
       </c>
       <c r="O48" s="6"/>
     </row>
@@ -3043,7 +3043,7 @@
       </c>
       <c r="N49" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">168, </v>
+        <v xml:space="preserve">167, </v>
       </c>
     </row>
     <row r="50" spans="5:14" x14ac:dyDescent="0.35">
@@ -3084,7 +3084,7 @@
       </c>
       <c r="N50" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">201, </v>
+        <v xml:space="preserve">200, </v>
       </c>
     </row>
     <row r="51" spans="5:14" x14ac:dyDescent="0.35">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="N51" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">242, 
+        <v xml:space="preserve">241, 
 </v>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="N52" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">146, </v>
+        <v xml:space="preserve">145, </v>
       </c>
     </row>
     <row r="53" spans="5:14" x14ac:dyDescent="0.35">
@@ -3208,7 +3208,7 @@
       </c>
       <c r="N53" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">178, </v>
+        <v xml:space="preserve">177, </v>
       </c>
     </row>
     <row r="54" spans="5:14" x14ac:dyDescent="0.35">
@@ -3249,7 +3249,7 @@
       </c>
       <c r="N54" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">215, 
+        <v xml:space="preserve">214, 
 </v>
       </c>
     </row>
@@ -3291,7 +3291,7 @@
       </c>
       <c r="N55" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">132, </v>
+        <v xml:space="preserve">131, </v>
       </c>
     </row>
     <row r="56" spans="5:14" x14ac:dyDescent="0.35">
@@ -3332,7 +3332,7 @@
       </c>
       <c r="N56" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">161, </v>
+        <v xml:space="preserve">160, </v>
       </c>
     </row>
     <row r="57" spans="5:14" x14ac:dyDescent="0.35">
@@ -3373,7 +3373,7 @@
       </c>
       <c r="N57" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">195, </v>
+        <v xml:space="preserve">194, </v>
       </c>
     </row>
     <row r="58" spans="5:14" x14ac:dyDescent="0.35">
@@ -3414,7 +3414,7 @@
       </c>
       <c r="N58" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">239, 
+        <v xml:space="preserve">238, 
 </v>
       </c>
     </row>
@@ -3456,7 +3456,7 @@
       </c>
       <c r="N59" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">146, </v>
+        <v xml:space="preserve">145, </v>
       </c>
     </row>
     <row r="60" spans="5:14" x14ac:dyDescent="0.35">
@@ -3497,7 +3497,7 @@
       </c>
       <c r="N60" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">176, </v>
+        <v xml:space="preserve">175, </v>
       </c>
     </row>
     <row r="61" spans="5:14" x14ac:dyDescent="0.35">
@@ -3538,7 +3538,7 @@
       </c>
       <c r="N61" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">210, </v>
+        <v xml:space="preserve">209, </v>
       </c>
     </row>
     <row r="62" spans="5:14" x14ac:dyDescent="0.35">
@@ -3579,7 +3579,7 @@
       </c>
       <c r="N62" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">251, 
+        <v xml:space="preserve">250, 
 </v>
       </c>
     </row>
@@ -3621,7 +3621,7 @@
       </c>
       <c r="N63" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">151, </v>
+        <v xml:space="preserve">150, </v>
       </c>
     </row>
     <row r="64" spans="5:14" x14ac:dyDescent="0.35">
@@ -3662,7 +3662,7 @@
       </c>
       <c r="N64" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">183, </v>
+        <v xml:space="preserve">182, </v>
       </c>
     </row>
     <row r="65" spans="5:14" x14ac:dyDescent="0.35">
@@ -3703,7 +3703,7 @@
       </c>
       <c r="N65" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">222, 
+        <v xml:space="preserve">221, 
 </v>
       </c>
     </row>
@@ -3745,7 +3745,7 @@
       </c>
       <c r="N66" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">134, </v>
+        <v xml:space="preserve">133, </v>
       </c>
     </row>
     <row r="67" spans="5:14" x14ac:dyDescent="0.35">
@@ -3786,7 +3786,7 @@
       </c>
       <c r="N67" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">165, </v>
+        <v xml:space="preserve">164, </v>
       </c>
     </row>
     <row r="68" spans="5:14" x14ac:dyDescent="0.35">
@@ -3827,7 +3827,7 @@
       </c>
       <c r="N68" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">201, </v>
+        <v xml:space="preserve">200, </v>
       </c>
     </row>
     <row r="69" spans="5:14" x14ac:dyDescent="0.35">
@@ -3868,7 +3868,7 @@
       </c>
       <c r="N69" s="19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">244, 
+        <v xml:space="preserve">243, 
 </v>
       </c>
     </row>
@@ -3909,8 +3909,8 @@
         <v xml:space="preserve">83, </v>
       </c>
       <c r="N70" s="19" t="str">
-        <f t="shared" ref="N70:N79" si="18">IF(J70&lt;&gt;"",J70&amp;", "&amp;IF($H70&lt;&gt;$H71,CHAR(10),""),256^$C$8-1&amp;CHAR(10))</f>
-        <v xml:space="preserve">150, </v>
+        <f t="shared" ref="N70:N79" si="18">IF(J70&lt;&gt;"",J70-1&amp;", "&amp;IF($H70&lt;&gt;$H71,CHAR(10),""),256^$C$8-1&amp;CHAR(10))</f>
+        <v xml:space="preserve">149, </v>
       </c>
     </row>
     <row r="71" spans="5:14" x14ac:dyDescent="0.35">
@@ -3951,7 +3951,7 @@
       </c>
       <c r="N71" s="19" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">183, </v>
+        <v xml:space="preserve">182, </v>
       </c>
     </row>
     <row r="72" spans="5:14" x14ac:dyDescent="0.35">
@@ -3992,7 +3992,7 @@
       </c>
       <c r="N72" s="19" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">220, 
+        <v xml:space="preserve">219, 
 </v>
       </c>
     </row>
@@ -4034,7 +4034,7 @@
       </c>
       <c r="N73" s="19" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">131, </v>
+        <v xml:space="preserve">130, </v>
       </c>
     </row>
     <row r="74" spans="5:14" x14ac:dyDescent="0.35">
@@ -4075,7 +4075,7 @@
       </c>
       <c r="N74" s="19" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">157, </v>
+        <v xml:space="preserve">156, </v>
       </c>
     </row>
     <row r="75" spans="5:14" x14ac:dyDescent="0.35">
@@ -4116,7 +4116,7 @@
       </c>
       <c r="N75" s="19" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">189, </v>
+        <v xml:space="preserve">188, </v>
       </c>
     </row>
     <row r="76" spans="5:14" x14ac:dyDescent="0.35">
@@ -4157,7 +4157,7 @@
       </c>
       <c r="N76" s="19" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">229, 
+        <v xml:space="preserve">228, 
 </v>
       </c>
     </row>
@@ -4199,7 +4199,7 @@
       </c>
       <c r="N77" s="19" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">139, </v>
+        <v xml:space="preserve">138, </v>
       </c>
     </row>
     <row r="78" spans="5:14" x14ac:dyDescent="0.35">
@@ -4240,7 +4240,7 @@
       </c>
       <c r="N78" s="19" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">168, 
+        <v xml:space="preserve">167, 
 </v>
       </c>
     </row>

</xml_diff>